<commit_message>
fixed an issue in compileProcedure for Kenzie. Heavy editing to updateTeachingMatLinks to add in gID in each dataframe as it's created.
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattwilkins/mrw_synced/R/Nonshiny Github/galacticPubs/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3C20EEA-1999-1F4B-A891-87A53D703F8B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9AA9EA-0457-D849-900B-21283F804358}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rsrcSumm" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="198">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -943,6 +943,9 @@
   </si>
   <si>
     <t>path</t>
+  </si>
+  <si>
+    <t>filetype</t>
   </si>
 </sst>
 </file>
@@ -9309,9 +9312,9 @@
   </sheetPr>
   <dimension ref="A1:AC99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:G7"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -9346,7 +9349,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>32</v>
+        <v>197</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>33</v>
@@ -11115,9 +11118,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AA976"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
added gPresentLink to DL folder, removed shareLink
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mattwilkins/mrw_synced/R/Nonshiny Github/galacticPubs/meta/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B9AA9EA-0457-D849-900B-21283F804358}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202C1DB3-F056-1F43-A52C-645ACF8BB349}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="197">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -466,9 +466,6 @@
   </si>
   <si>
     <t>formShareLink</t>
-  </si>
-  <si>
-    <t>shareLink</t>
   </si>
   <si>
     <t>named_share_links</t>
@@ -1395,7 +1392,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1518,6 +1515,7 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="19" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2253,7 +2251,7 @@
     <row r="21" spans="1:11" ht="18" customHeight="1">
       <c r="A21" s="5"/>
       <c r="B21" s="41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="6"/>
       <c r="D21" s="5"/>
@@ -9310,11 +9308,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC99"/>
+  <dimension ref="A1:AC100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -9326,7 +9324,7 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="21.6640625" customWidth="1"/>
-    <col min="8" max="8" width="12.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21.5" style="32" customWidth="1"/>
     <col min="9" max="9" width="38.83203125" customWidth="1"/>
     <col min="11" max="11" width="21.6640625" customWidth="1"/>
   </cols>
@@ -9341,7 +9339,7 @@
       <c r="E1" s="83"/>
       <c r="F1" s="83"/>
       <c r="G1" s="83"/>
-      <c r="H1" s="83"/>
+      <c r="H1" s="86"/>
       <c r="I1" s="83"/>
     </row>
     <row r="2" spans="1:29" ht="18.75" customHeight="1">
@@ -9349,7 +9347,7 @@
         <v>31</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>33</v>
@@ -9366,11 +9364,11 @@
       <c r="G2" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="29" t="s">
+        <v>43</v>
+      </c>
+      <c r="I2" s="12" t="s">
         <v>38</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>39</v>
       </c>
       <c r="J2" s="15"/>
       <c r="K2" s="15"/>
@@ -9397,24 +9395,21 @@
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E3" s="81" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G3" s="18"/>
-      <c r="H3" s="19" t="str">
-        <f t="shared" ref="H3:H34" si="0">IF(ISBLANK(E3),"",(MID(E3,1,SEARCH("/edit",E3))&amp;"present"))</f>
-        <v/>
-      </c>
+      <c r="H3" s="33"/>
       <c r="I3" s="20" t="str">
-        <f t="shared" ref="I3:I34" si="1">IF(H3="","",HYPERLINK(H3,IF(B3="feedback-form",B3,B3&amp;"_(part-"&amp;C3&amp;")")))</f>
+        <f>IF(H3="","",HYPERLINK(H3,IF(B3="feedback-form",B3,B3&amp;"_(part-"&amp;C3&amp;")")))</f>
         <v/>
       </c>
     </row>
@@ -9422,24 +9417,21 @@
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="81" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G4" s="18"/>
-      <c r="H4" s="19" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
+      <c r="H4" s="33"/>
       <c r="I4" s="20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="I4:I67" si="0">IF(H4="","",HYPERLINK(H4,IF(B4="feedback-form",B4,B4&amp;"_(part-"&amp;C4&amp;")")))</f>
         <v/>
       </c>
     </row>
@@ -9447,24 +9439,21 @@
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="81" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F5" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5" s="18"/>
-      <c r="H5" s="19" t="str">
+      <c r="H5" s="33"/>
+      <c r="I5" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I5" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9473,21 +9462,18 @@
       <c r="B6" s="16"/>
       <c r="C6" s="23"/>
       <c r="D6" s="81" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E6" s="81" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F6" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="18"/>
-      <c r="H6" s="19" t="str">
+      <c r="H6" s="33"/>
+      <c r="I6" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I6" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9496,21 +9482,18 @@
       <c r="B7" s="16"/>
       <c r="C7" s="23"/>
       <c r="D7" s="81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E7" s="81" t="s">
+        <v>83</v>
+      </c>
+      <c r="F7" s="81" t="s">
         <v>84</v>
       </c>
-      <c r="F7" s="81" t="s">
-        <v>85</v>
-      </c>
       <c r="G7" s="18"/>
-      <c r="H7" s="19" t="str">
+      <c r="H7" s="33"/>
+      <c r="I7" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I7" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9522,12 +9505,9 @@
       <c r="E8" s="23"/>
       <c r="F8" s="17"/>
       <c r="G8" s="18"/>
-      <c r="H8" s="19" t="str">
+      <c r="H8" s="33"/>
+      <c r="I8" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I8" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9539,12 +9519,9 @@
       <c r="E9" s="23"/>
       <c r="F9" s="17"/>
       <c r="G9" s="18"/>
-      <c r="H9" s="19" t="str">
+      <c r="H9" s="33"/>
+      <c r="I9" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I9" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9556,12 +9533,9 @@
       <c r="E10" s="23"/>
       <c r="F10" s="17"/>
       <c r="G10" s="18"/>
-      <c r="H10" s="19" t="str">
+      <c r="H10" s="33"/>
+      <c r="I10" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I10" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9573,12 +9547,9 @@
       <c r="E11" s="23"/>
       <c r="F11" s="17"/>
       <c r="G11" s="18"/>
-      <c r="H11" s="19" t="str">
+      <c r="H11" s="33"/>
+      <c r="I11" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I11" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9590,12 +9561,9 @@
       <c r="E12" s="23"/>
       <c r="F12" s="17"/>
       <c r="G12" s="18"/>
-      <c r="H12" s="19" t="str">
+      <c r="H12" s="33"/>
+      <c r="I12" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I12" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9607,12 +9575,9 @@
       <c r="E13" s="23"/>
       <c r="F13" s="17"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="19" t="str">
+      <c r="H13" s="33"/>
+      <c r="I13" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I13" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9624,12 +9589,9 @@
       <c r="E14" s="23"/>
       <c r="F14" s="17"/>
       <c r="G14" s="18"/>
-      <c r="H14" s="19" t="str">
+      <c r="H14" s="33"/>
+      <c r="I14" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I14" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9641,12 +9603,9 @@
       <c r="E15" s="23"/>
       <c r="F15" s="17"/>
       <c r="G15" s="18"/>
-      <c r="H15" s="19" t="str">
+      <c r="H15" s="33"/>
+      <c r="I15" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I15" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9658,12 +9617,9 @@
       <c r="E16" s="23"/>
       <c r="F16" s="17"/>
       <c r="G16" s="18"/>
-      <c r="H16" s="19" t="str">
+      <c r="H16" s="33"/>
+      <c r="I16" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I16" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9675,12 +9631,9 @@
       <c r="E17" s="23"/>
       <c r="F17" s="17"/>
       <c r="G17" s="18"/>
-      <c r="H17" s="19" t="str">
+      <c r="H17" s="33"/>
+      <c r="I17" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I17" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9692,12 +9645,9 @@
       <c r="E18" s="23"/>
       <c r="F18" s="17"/>
       <c r="G18" s="18"/>
-      <c r="H18" s="19" t="str">
+      <c r="H18" s="33"/>
+      <c r="I18" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I18" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9709,12 +9659,9 @@
       <c r="E19" s="23"/>
       <c r="F19" s="17"/>
       <c r="G19" s="18"/>
-      <c r="H19" s="19" t="str">
+      <c r="H19" s="33"/>
+      <c r="I19" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I19" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9726,12 +9673,9 @@
       <c r="E20" s="23"/>
       <c r="F20" s="17"/>
       <c r="G20" s="18"/>
-      <c r="H20" s="19" t="str">
+      <c r="H20" s="33"/>
+      <c r="I20" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I20" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9743,12 +9687,9 @@
       <c r="E21" s="23"/>
       <c r="F21" s="17"/>
       <c r="G21" s="18"/>
-      <c r="H21" s="19" t="str">
+      <c r="H21" s="33"/>
+      <c r="I21" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I21" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9760,12 +9701,9 @@
       <c r="E22" s="23"/>
       <c r="F22" s="17"/>
       <c r="G22" s="18"/>
-      <c r="H22" s="19" t="str">
+      <c r="H22" s="33"/>
+      <c r="I22" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I22" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9777,12 +9715,9 @@
       <c r="E23" s="23"/>
       <c r="F23" s="17"/>
       <c r="G23" s="18"/>
-      <c r="H23" s="19" t="str">
+      <c r="H23" s="33"/>
+      <c r="I23" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I23" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9794,12 +9729,9 @@
       <c r="E24" s="23"/>
       <c r="F24" s="17"/>
       <c r="G24" s="18"/>
-      <c r="H24" s="19" t="str">
+      <c r="H24" s="33"/>
+      <c r="I24" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I24" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9811,12 +9743,9 @@
       <c r="E25" s="23"/>
       <c r="F25" s="17"/>
       <c r="G25" s="18"/>
-      <c r="H25" s="19" t="str">
+      <c r="H25" s="33"/>
+      <c r="I25" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I25" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9828,12 +9757,9 @@
       <c r="E26" s="23"/>
       <c r="F26" s="17"/>
       <c r="G26" s="18"/>
-      <c r="H26" s="19" t="str">
+      <c r="H26" s="33"/>
+      <c r="I26" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I26" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9845,12 +9771,9 @@
       <c r="E27" s="23"/>
       <c r="F27" s="17"/>
       <c r="G27" s="18"/>
-      <c r="H27" s="19" t="str">
+      <c r="H27" s="33"/>
+      <c r="I27" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I27" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9862,12 +9785,9 @@
       <c r="E28" s="23"/>
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
-      <c r="H28" s="19" t="str">
+      <c r="H28" s="33"/>
+      <c r="I28" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I28" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9879,12 +9799,9 @@
       <c r="E29" s="23"/>
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
-      <c r="H29" s="19" t="str">
+      <c r="H29" s="33"/>
+      <c r="I29" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I29" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9896,12 +9813,9 @@
       <c r="E30" s="23"/>
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
-      <c r="H30" s="19" t="str">
+      <c r="H30" s="33"/>
+      <c r="I30" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I30" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9913,12 +9827,9 @@
       <c r="E31" s="23"/>
       <c r="F31" s="17"/>
       <c r="G31" s="18"/>
-      <c r="H31" s="19" t="str">
+      <c r="H31" s="33"/>
+      <c r="I31" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I31" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9930,12 +9841,9 @@
       <c r="E32" s="23"/>
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
-      <c r="H32" s="19" t="str">
+      <c r="H32" s="33"/>
+      <c r="I32" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I32" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9947,12 +9855,9 @@
       <c r="E33" s="23"/>
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
-      <c r="H33" s="19" t="str">
+      <c r="H33" s="33"/>
+      <c r="I33" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I33" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9964,12 +9869,9 @@
       <c r="E34" s="23"/>
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
-      <c r="H34" s="19" t="str">
+      <c r="H34" s="33"/>
+      <c r="I34" s="20" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="I34" s="20" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -9981,12 +9883,9 @@
       <c r="E35" s="23"/>
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
-      <c r="H35" s="19" t="str">
-        <f t="shared" ref="H35:H66" si="2">IF(ISBLANK(E35),"",(MID(E35,1,SEARCH("/edit",E35))&amp;"present"))</f>
-        <v/>
-      </c>
+      <c r="H35" s="33"/>
       <c r="I35" s="20" t="str">
-        <f t="shared" ref="I35:I66" si="3">IF(H35="","",HYPERLINK(H35,IF(B35="feedback-form",B35,B35&amp;"_(part-"&amp;C35&amp;")")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -9998,12 +9897,9 @@
       <c r="E36" s="23"/>
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
-      <c r="H36" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H36" s="33"/>
       <c r="I36" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10015,12 +9911,9 @@
       <c r="E37" s="23"/>
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
-      <c r="H37" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H37" s="33"/>
       <c r="I37" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10032,12 +9925,9 @@
       <c r="E38" s="23"/>
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
-      <c r="H38" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H38" s="33"/>
       <c r="I38" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10049,12 +9939,9 @@
       <c r="E39" s="23"/>
       <c r="F39" s="17"/>
       <c r="G39" s="18"/>
-      <c r="H39" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H39" s="33"/>
       <c r="I39" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10066,12 +9953,9 @@
       <c r="E40" s="23"/>
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
-      <c r="H40" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H40" s="33"/>
       <c r="I40" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10083,12 +9967,9 @@
       <c r="E41" s="23"/>
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
-      <c r="H41" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H41" s="33"/>
       <c r="I41" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10100,12 +9981,9 @@
       <c r="E42" s="23"/>
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
-      <c r="H42" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H42" s="33"/>
       <c r="I42" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10117,12 +9995,9 @@
       <c r="E43" s="23"/>
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
-      <c r="H43" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H43" s="33"/>
       <c r="I43" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10134,12 +10009,9 @@
       <c r="E44" s="23"/>
       <c r="F44" s="17"/>
       <c r="G44" s="18"/>
-      <c r="H44" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H44" s="33"/>
       <c r="I44" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10151,12 +10023,9 @@
       <c r="E45" s="23"/>
       <c r="F45" s="17"/>
       <c r="G45" s="18"/>
-      <c r="H45" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H45" s="33"/>
       <c r="I45" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10168,12 +10037,9 @@
       <c r="E46" s="23"/>
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
-      <c r="H46" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H46" s="33"/>
       <c r="I46" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10185,12 +10051,9 @@
       <c r="E47" s="23"/>
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
-      <c r="H47" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H47" s="33"/>
       <c r="I47" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10202,12 +10065,9 @@
       <c r="E48" s="23"/>
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
-      <c r="H48" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H48" s="33"/>
       <c r="I48" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10219,12 +10079,9 @@
       <c r="E49" s="23"/>
       <c r="F49" s="17"/>
       <c r="G49" s="18"/>
-      <c r="H49" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H49" s="33"/>
       <c r="I49" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10236,12 +10093,9 @@
       <c r="E50" s="23"/>
       <c r="F50" s="17"/>
       <c r="G50" s="18"/>
-      <c r="H50" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H50" s="33"/>
       <c r="I50" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10253,12 +10107,9 @@
       <c r="E51" s="23"/>
       <c r="F51" s="17"/>
       <c r="G51" s="18"/>
-      <c r="H51" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H51" s="33"/>
       <c r="I51" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10270,12 +10121,9 @@
       <c r="E52" s="23"/>
       <c r="F52" s="17"/>
       <c r="G52" s="18"/>
-      <c r="H52" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H52" s="33"/>
       <c r="I52" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10287,12 +10135,9 @@
       <c r="E53" s="23"/>
       <c r="F53" s="17"/>
       <c r="G53" s="18"/>
-      <c r="H53" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H53" s="33"/>
       <c r="I53" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10304,12 +10149,9 @@
       <c r="E54" s="23"/>
       <c r="F54" s="17"/>
       <c r="G54" s="18"/>
-      <c r="H54" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H54" s="33"/>
       <c r="I54" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10321,12 +10163,9 @@
       <c r="E55" s="23"/>
       <c r="F55" s="17"/>
       <c r="G55" s="18"/>
-      <c r="H55" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H55" s="33"/>
       <c r="I55" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10338,12 +10177,9 @@
       <c r="E56" s="23"/>
       <c r="F56" s="17"/>
       <c r="G56" s="18"/>
-      <c r="H56" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H56" s="33"/>
       <c r="I56" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10355,12 +10191,9 @@
       <c r="E57" s="23"/>
       <c r="F57" s="17"/>
       <c r="G57" s="18"/>
-      <c r="H57" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H57" s="33"/>
       <c r="I57" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10372,12 +10205,9 @@
       <c r="E58" s="23"/>
       <c r="F58" s="17"/>
       <c r="G58" s="18"/>
-      <c r="H58" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H58" s="33"/>
       <c r="I58" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10389,12 +10219,9 @@
       <c r="E59" s="23"/>
       <c r="F59" s="17"/>
       <c r="G59" s="18"/>
-      <c r="H59" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H59" s="33"/>
       <c r="I59" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10406,12 +10233,9 @@
       <c r="E60" s="23"/>
       <c r="F60" s="17"/>
       <c r="G60" s="18"/>
-      <c r="H60" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H60" s="33"/>
       <c r="I60" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10423,12 +10247,9 @@
       <c r="E61" s="23"/>
       <c r="F61" s="17"/>
       <c r="G61" s="18"/>
-      <c r="H61" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H61" s="33"/>
       <c r="I61" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10440,12 +10261,9 @@
       <c r="E62" s="23"/>
       <c r="F62" s="17"/>
       <c r="G62" s="18"/>
-      <c r="H62" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H62" s="33"/>
       <c r="I62" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10457,12 +10275,9 @@
       <c r="E63" s="23"/>
       <c r="F63" s="17"/>
       <c r="G63" s="18"/>
-      <c r="H63" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H63" s="33"/>
       <c r="I63" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10474,12 +10289,9 @@
       <c r="E64" s="23"/>
       <c r="F64" s="17"/>
       <c r="G64" s="18"/>
-      <c r="H64" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H64" s="33"/>
       <c r="I64" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10491,12 +10303,9 @@
       <c r="E65" s="23"/>
       <c r="F65" s="17"/>
       <c r="G65" s="18"/>
-      <c r="H65" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H65" s="33"/>
       <c r="I65" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10508,12 +10317,9 @@
       <c r="E66" s="23"/>
       <c r="F66" s="17"/>
       <c r="G66" s="18"/>
-      <c r="H66" s="19" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
+      <c r="H66" s="33"/>
       <c r="I66" s="20" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10525,12 +10331,9 @@
       <c r="E67" s="23"/>
       <c r="F67" s="17"/>
       <c r="G67" s="18"/>
-      <c r="H67" s="19" t="str">
-        <f t="shared" ref="H67:H99" si="4">IF(ISBLANK(E67),"",(MID(E67,1,SEARCH("/edit",E67))&amp;"present"))</f>
-        <v/>
-      </c>
+      <c r="H67" s="33"/>
       <c r="I67" s="20" t="str">
-        <f t="shared" ref="I67:I98" si="5">IF(H67="","",HYPERLINK(H67,IF(B67="feedback-form",B67,B67&amp;"_(part-"&amp;C67&amp;")")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
@@ -10542,12 +10345,9 @@
       <c r="E68" s="23"/>
       <c r="F68" s="17"/>
       <c r="G68" s="18"/>
-      <c r="H68" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H68" s="33"/>
       <c r="I68" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="I68:I99" si="1">IF(H68="","",HYPERLINK(H68,IF(B68="feedback-form",B68,B68&amp;"_(part-"&amp;C68&amp;")")))</f>
         <v/>
       </c>
     </row>
@@ -10559,12 +10359,9 @@
       <c r="E69" s="23"/>
       <c r="F69" s="17"/>
       <c r="G69" s="18"/>
-      <c r="H69" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H69" s="33"/>
       <c r="I69" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10576,12 +10373,9 @@
       <c r="E70" s="23"/>
       <c r="F70" s="17"/>
       <c r="G70" s="18"/>
-      <c r="H70" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H70" s="33"/>
       <c r="I70" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10593,12 +10387,9 @@
       <c r="E71" s="23"/>
       <c r="F71" s="17"/>
       <c r="G71" s="18"/>
-      <c r="H71" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H71" s="33"/>
       <c r="I71" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10610,12 +10401,9 @@
       <c r="E72" s="23"/>
       <c r="F72" s="17"/>
       <c r="G72" s="18"/>
-      <c r="H72" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H72" s="33"/>
       <c r="I72" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10627,12 +10415,9 @@
       <c r="E73" s="23"/>
       <c r="F73" s="17"/>
       <c r="G73" s="18"/>
-      <c r="H73" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H73" s="33"/>
       <c r="I73" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10644,12 +10429,9 @@
       <c r="E74" s="23"/>
       <c r="F74" s="17"/>
       <c r="G74" s="18"/>
-      <c r="H74" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H74" s="33"/>
       <c r="I74" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10661,12 +10443,9 @@
       <c r="E75" s="23"/>
       <c r="F75" s="17"/>
       <c r="G75" s="18"/>
-      <c r="H75" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H75" s="33"/>
       <c r="I75" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10678,12 +10457,9 @@
       <c r="E76" s="23"/>
       <c r="F76" s="17"/>
       <c r="G76" s="18"/>
-      <c r="H76" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H76" s="33"/>
       <c r="I76" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10695,12 +10471,9 @@
       <c r="E77" s="23"/>
       <c r="F77" s="17"/>
       <c r="G77" s="18"/>
-      <c r="H77" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H77" s="33"/>
       <c r="I77" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10712,12 +10485,9 @@
       <c r="E78" s="23"/>
       <c r="F78" s="17"/>
       <c r="G78" s="18"/>
-      <c r="H78" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H78" s="33"/>
       <c r="I78" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10729,12 +10499,9 @@
       <c r="E79" s="23"/>
       <c r="F79" s="17"/>
       <c r="G79" s="18"/>
-      <c r="H79" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H79" s="33"/>
       <c r="I79" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10746,12 +10513,9 @@
       <c r="E80" s="23"/>
       <c r="F80" s="17"/>
       <c r="G80" s="18"/>
-      <c r="H80" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H80" s="33"/>
       <c r="I80" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10763,12 +10527,9 @@
       <c r="E81" s="23"/>
       <c r="F81" s="17"/>
       <c r="G81" s="18"/>
-      <c r="H81" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H81" s="33"/>
       <c r="I81" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10780,12 +10541,9 @@
       <c r="E82" s="23"/>
       <c r="F82" s="17"/>
       <c r="G82" s="18"/>
-      <c r="H82" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H82" s="33"/>
       <c r="I82" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10797,12 +10555,9 @@
       <c r="E83" s="23"/>
       <c r="F83" s="17"/>
       <c r="G83" s="18"/>
-      <c r="H83" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H83" s="33"/>
       <c r="I83" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10814,12 +10569,9 @@
       <c r="E84" s="23"/>
       <c r="F84" s="17"/>
       <c r="G84" s="18"/>
-      <c r="H84" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H84" s="33"/>
       <c r="I84" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10831,12 +10583,9 @@
       <c r="E85" s="23"/>
       <c r="F85" s="17"/>
       <c r="G85" s="18"/>
-      <c r="H85" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H85" s="33"/>
       <c r="I85" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10848,12 +10597,9 @@
       <c r="E86" s="23"/>
       <c r="F86" s="17"/>
       <c r="G86" s="18"/>
-      <c r="H86" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H86" s="33"/>
       <c r="I86" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10865,12 +10611,9 @@
       <c r="E87" s="23"/>
       <c r="F87" s="17"/>
       <c r="G87" s="18"/>
-      <c r="H87" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H87" s="33"/>
       <c r="I87" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10882,12 +10625,9 @@
       <c r="E88" s="23"/>
       <c r="F88" s="17"/>
       <c r="G88" s="18"/>
-      <c r="H88" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H88" s="33"/>
       <c r="I88" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10899,12 +10639,9 @@
       <c r="E89" s="23"/>
       <c r="F89" s="17"/>
       <c r="G89" s="18"/>
-      <c r="H89" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H89" s="33"/>
       <c r="I89" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10916,12 +10653,9 @@
       <c r="E90" s="23"/>
       <c r="F90" s="17"/>
       <c r="G90" s="18"/>
-      <c r="H90" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H90" s="33"/>
       <c r="I90" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10933,12 +10667,9 @@
       <c r="E91" s="23"/>
       <c r="F91" s="17"/>
       <c r="G91" s="18"/>
-      <c r="H91" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H91" s="33"/>
       <c r="I91" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10950,12 +10681,9 @@
       <c r="E92" s="23"/>
       <c r="F92" s="17"/>
       <c r="G92" s="18"/>
-      <c r="H92" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H92" s="33"/>
       <c r="I92" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10967,12 +10695,9 @@
       <c r="E93" s="23"/>
       <c r="F93" s="17"/>
       <c r="G93" s="18"/>
-      <c r="H93" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H93" s="33"/>
       <c r="I93" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -10984,12 +10709,9 @@
       <c r="E94" s="23"/>
       <c r="F94" s="17"/>
       <c r="G94" s="18"/>
-      <c r="H94" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H94" s="33"/>
       <c r="I94" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -11001,12 +10723,9 @@
       <c r="E95" s="23"/>
       <c r="F95" s="17"/>
       <c r="G95" s="18"/>
-      <c r="H95" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H95" s="33"/>
       <c r="I95" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -11018,12 +10737,9 @@
       <c r="E96" s="23"/>
       <c r="F96" s="17"/>
       <c r="G96" s="18"/>
-      <c r="H96" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H96" s="33"/>
       <c r="I96" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -11035,12 +10751,9 @@
       <c r="E97" s="23"/>
       <c r="F97" s="17"/>
       <c r="G97" s="18"/>
-      <c r="H97" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H97" s="33"/>
       <c r="I97" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -11052,12 +10765,9 @@
       <c r="E98" s="23"/>
       <c r="F98" s="17"/>
       <c r="G98" s="18"/>
-      <c r="H98" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H98" s="33"/>
       <c r="I98" s="20" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -11069,14 +10779,14 @@
       <c r="E99" s="23"/>
       <c r="F99" s="17"/>
       <c r="G99" s="18"/>
-      <c r="H99" s="19" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="H99" s="33"/>
       <c r="I99" s="20" t="str">
-        <f t="shared" ref="I99" si="6">IF(H99="","",HYPERLINK(H99,IF(B99="feedback-form",B99,B99&amp;"_(part-"&amp;C99&amp;")")))</f>
-        <v/>
-      </c>
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="15" customHeight="1">
+      <c r="H100" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:I99" xr:uid="{00000000-0009-0000-0000-000001000000}">
@@ -11135,8 +10845,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19.5" customHeight="1">
-      <c r="A1" s="86" t="s">
-        <v>40</v>
+      <c r="A1" s="87" t="s">
+        <v>39</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -11149,13 +10859,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>33</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>35</v>
@@ -11190,19 +10900,19 @@
         <v>6</v>
       </c>
       <c r="B3" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="81" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F3" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G3" s="24"/>
       <c r="H3" s="24"/>
@@ -11222,19 +10932,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E4" s="81" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F4" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
@@ -11254,19 +10964,19 @@
         <v>6</v>
       </c>
       <c r="B5" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D5" s="81" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E5" s="81" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F5" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
@@ -11286,19 +10996,19 @@
         <v>6</v>
       </c>
       <c r="B6" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C6" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E6" s="81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
@@ -11318,19 +11028,19 @@
         <v>20</v>
       </c>
       <c r="B7" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="81" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F7" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G7" s="24"/>
       <c r="H7" s="24"/>
@@ -11350,19 +11060,19 @@
         <v>20</v>
       </c>
       <c r="B8" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E8" s="81" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F8" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G8" s="24"/>
       <c r="H8" s="24"/>
@@ -11382,19 +11092,19 @@
         <v>20</v>
       </c>
       <c r="B9" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D9" s="81" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E9" s="81" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F9" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G9" s="24"/>
       <c r="H9" s="24"/>
@@ -11414,19 +11124,19 @@
         <v>20</v>
       </c>
       <c r="B10" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="81" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D10" s="81" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E10" s="81" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G10" s="24"/>
       <c r="H10" s="24"/>
@@ -18737,7 +18447,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:G12"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -18756,8 +18466,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1">
-      <c r="A1" s="87" t="s">
-        <v>42</v>
+      <c r="A1" s="88" t="s">
+        <v>41</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -18799,7 +18509,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>33</v>
@@ -18814,13 +18524,13 @@
         <v>36</v>
       </c>
       <c r="H2" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="J2" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="K2" s="30"/>
       <c r="L2" s="31"/>
@@ -18829,19 +18539,19 @@
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="81" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F3" s="81" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G3" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H3" s="19" t="str">
         <f t="shared" ref="H3:H11" si="0">IF(ISBLANK($F3),"",(MID($F3,1,SEARCH("/edit",$F3))&amp;"template/preview"))</f>
@@ -18862,19 +18572,19 @@
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" s="81" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F4" s="81" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G4" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H4" s="19" t="str">
         <f t="shared" si="0"/>
@@ -18895,19 +18605,19 @@
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="81" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F5" s="81" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G5" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="19" t="str">
         <f t="shared" si="0"/>
@@ -18928,19 +18638,19 @@
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E6" s="81" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F6" s="81" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="19" t="str">
         <f t="shared" si="0"/>
@@ -18961,19 +18671,19 @@
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="81" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F7" s="81" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G7" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H7" s="19" t="str">
         <f t="shared" si="0"/>
@@ -18994,19 +18704,19 @@
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="81" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="81" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G8" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H8" s="19" t="str">
         <f t="shared" si="0"/>
@@ -19027,19 +18737,19 @@
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D9" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="81" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F9" s="81" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G9" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H9" s="19" t="str">
         <f t="shared" si="0"/>
@@ -19060,19 +18770,19 @@
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D10" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E10" s="81" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F10" s="81" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G10" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H10" s="19" t="str">
         <f t="shared" si="0"/>
@@ -19093,19 +18803,19 @@
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D11" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E11" s="81" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="81" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G11" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H11" s="19" t="str">
         <f t="shared" si="0"/>
@@ -20926,9 +20636,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AE99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -20948,8 +20658,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.5" customHeight="1">
-      <c r="A1" s="88" t="s">
-        <v>46</v>
+      <c r="A1" s="89" t="s">
+        <v>45</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -20990,16 +20700,16 @@
         <v>32</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="40" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" s="40" t="s">
-        <v>48</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>34</v>
@@ -21011,10 +20721,10 @@
         <v>36</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="41"/>
@@ -21041,23 +20751,23 @@
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="81" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H3" s="81" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I3" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J3" s="43" t="str">
         <f t="shared" ref="J3:J99" si="0">IF(ISBLANK(H3),"",HYPERLINK(MID(H3,1,SEARCH("/edit",H3))&amp;"template/preview"))</f>
@@ -21065,7 +20775,7 @@
       </c>
       <c r="K3" s="44" t="str">
         <f t="shared" ref="K3:K22" si="1">IF(ISBLANK(H3),"",HYPERLINK(MID(H3,1,SEARCH("/edit",H3))&amp;"export?format=pdf"))</f>
-        <v/>
+        <v>https://docs.google.com/document/d/16f_VJ2xCNy2qzs4majLlMbVDzf93pYYXTkKmcqwr9kc/export?format=pdf</v>
       </c>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
@@ -21088,23 +20798,23 @@
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="81" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H4" s="81" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I4" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J4" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21135,23 +20845,23 @@
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E5" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="81" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H5" s="81" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I5" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J5" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21182,21 +20892,21 @@
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="81" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H6" s="81" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I6" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J6" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21227,23 +20937,23 @@
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="81" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H7" s="81" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="I7" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J7" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21274,31 +20984,31 @@
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="81" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H8" s="81" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I8" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J8" s="43" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K8" s="44" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+        <f>IF(ISBLANK(H8),"",HYPERLINK(MID(H8,1,SEARCH("/edit",H8))&amp;"export?format=pdf"))</f>
+        <v>https://docs.google.com/document/d/1a9PDt1ImC0JG7_vZqh-yXcCa7RYBa-DqyRfbqRDZsVE/export?format=pdf</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
@@ -21321,23 +21031,23 @@
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F9" s="16"/>
       <c r="G9" s="81" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H9" s="81" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="I9" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J9" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21368,27 +21078,27 @@
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E10" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="81" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H10" s="81" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="I10" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J10" s="43" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+        <f>IF(ISBLANK(H10),"",HYPERLINK(MID(H10,1,SEARCH("/edit",H10))&amp;"template/preview"))</f>
+        <v>https://docs.google.com/document/d/1ccHAO3mwI59t38HbyyCYEyKrrPGjO9rljQojC9vFmic/template/preview</v>
       </c>
       <c r="K10" s="44" t="str">
         <f t="shared" si="1"/>
@@ -21415,23 +21125,23 @@
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
       <c r="C11" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D11" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="81" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H11" s="81" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="I11" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J11" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21462,23 +21172,23 @@
       <c r="A12" s="16"/>
       <c r="B12" s="16"/>
       <c r="C12" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E12" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="81" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H12" s="81" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="I12" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J12" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21509,21 +21219,21 @@
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="81" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H13" s="81" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="I13" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J13" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21554,23 +21264,23 @@
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D14" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E14" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="81" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H14" s="81" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="I14" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J14" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21601,23 +21311,23 @@
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D15" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E15" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F15" s="16"/>
       <c r="G15" s="81" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H15" s="81" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I15" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J15" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21648,23 +21358,23 @@
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D16" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E16" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F16" s="16"/>
       <c r="G16" s="81" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H16" s="81" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I16" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J16" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21695,23 +21405,23 @@
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D17" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E17" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="16"/>
       <c r="G17" s="81" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H17" s="81" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I17" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J17" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21742,23 +21452,23 @@
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D18" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E18" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" s="16"/>
       <c r="G18" s="81" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H18" s="81" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I18" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J18" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21789,23 +21499,23 @@
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D19" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E19" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F19" s="16"/>
       <c r="G19" s="81" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H19" s="81" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="I19" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J19" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21836,21 +21546,21 @@
       <c r="A20" s="16"/>
       <c r="B20" s="16"/>
       <c r="C20" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D20" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="81" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H20" s="81" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="I20" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J20" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21881,23 +21591,23 @@
       <c r="A21" s="16"/>
       <c r="B21" s="16"/>
       <c r="C21" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D21" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E21" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F21" s="16"/>
       <c r="G21" s="81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H21" s="81" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I21" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J21" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21928,23 +21638,23 @@
       <c r="A22" s="16"/>
       <c r="B22" s="16"/>
       <c r="C22" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D22" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E22" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F22" s="16"/>
       <c r="G22" s="81" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H22" s="81" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="I22" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J22" s="43" t="str">
         <f t="shared" si="0"/>
@@ -21975,23 +21685,23 @@
       <c r="A23" s="16"/>
       <c r="B23" s="16"/>
       <c r="C23" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D23" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E23" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F23" s="16"/>
       <c r="G23" s="81" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H23" s="81" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I23" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J23" s="43" t="str">
         <f t="shared" si="0"/>
@@ -24486,7 +24196,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -24507,8 +24217,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="21.75" customHeight="1">
-      <c r="A1" s="89" t="s">
-        <v>50</v>
+      <c r="A1" s="90" t="s">
+        <v>49</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -24531,7 +24241,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>33</v>
@@ -24546,16 +24256,16 @@
         <v>36</v>
       </c>
       <c r="H2" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" s="49" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="J2" s="50" t="s">
-        <v>52</v>
-      </c>
       <c r="K2" s="51" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L2" s="13"/>
       <c r="M2" s="14"/>
@@ -24584,19 +24294,19 @@
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="81" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F3" s="81" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G3" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H3" s="43" t="str">
         <f t="shared" ref="H3:H100" si="0">IF(ISBLANK(F3),"",HYPERLINK(MID(F3,1,SEARCH("/edit",F3))&amp;"template/preview"))</f>
@@ -24616,19 +24326,19 @@
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E4" s="81" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="F4" s="81" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G4" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H4" s="43" t="str">
         <f t="shared" si="0"/>
@@ -24647,19 +24357,19 @@
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="81" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F5" s="81" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G5" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H5" s="43" t="str">
         <f t="shared" si="0"/>
@@ -24678,19 +24388,19 @@
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="81" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F6" s="81" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G6" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="43" t="str">
         <f t="shared" si="0"/>
@@ -24709,19 +24419,19 @@
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E7" s="81" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F7" s="81" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G7" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H7" s="43" t="str">
         <f t="shared" si="0"/>
@@ -24740,19 +24450,19 @@
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="81" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F8" s="81" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G8" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H8" s="43" t="str">
         <f t="shared" si="0"/>
@@ -24771,19 +24481,19 @@
       <c r="A9" s="16"/>
       <c r="B9" s="16"/>
       <c r="C9" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" s="81" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E9" s="81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F9" s="81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G9" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H9" s="43" t="str">
         <f t="shared" si="0"/>
@@ -24802,19 +24512,19 @@
       <c r="A10" s="16"/>
       <c r="B10" s="16"/>
       <c r="C10" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D10" s="81" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E10" s="81" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F10" s="81" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G10" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H10" s="43" t="str">
         <f t="shared" si="0"/>
@@ -24833,19 +24543,19 @@
       <c r="A11" s="23"/>
       <c r="B11" s="16"/>
       <c r="C11" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E11" s="81" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F11" s="81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G11" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H11" s="43" t="str">
         <f t="shared" si="0"/>
@@ -26769,8 +26479,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75" customHeight="1">
-      <c r="A1" s="89" t="s">
-        <v>53</v>
+      <c r="A1" s="90" t="s">
+        <v>52</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -26791,16 +26501,16 @@
         <v>32</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>33</v>
       </c>
       <c r="E2" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="10" t="s">
         <v>47</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>48</v>
       </c>
       <c r="G2" s="10" t="s">
         <v>34</v>
@@ -26812,10 +26522,10 @@
         <v>36</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="41"/>
@@ -26842,23 +26552,23 @@
       <c r="A3" s="16"/>
       <c r="B3" s="16"/>
       <c r="C3" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D3" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E3" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F3" s="16"/>
       <c r="G3" s="81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H3" s="81" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I3" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J3" s="63" t="str">
         <f t="shared" ref="J3:J100" si="0">IF($H3="","",HYPERLINK(MID($H3,1,SEARCH("/view",$H3))&amp;"template/preview"))</f>
@@ -26888,23 +26598,23 @@
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="81" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D4" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E4" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F4" s="16"/>
       <c r="G4" s="81" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H4" s="81" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I4" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J4" s="63" t="str">
         <f t="shared" si="0"/>
@@ -26934,23 +26644,23 @@
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F5" s="16"/>
       <c r="G5" s="81" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H5" s="81" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I5" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J5" s="63" t="str">
         <f t="shared" si="0"/>
@@ -26980,23 +26690,23 @@
       <c r="A6" s="16"/>
       <c r="B6" s="16"/>
       <c r="C6" s="81" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E6" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F6" s="16"/>
       <c r="G6" s="81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H6" s="81" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="I6" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J6" s="63" t="str">
         <f t="shared" si="0"/>
@@ -27026,23 +26736,23 @@
       <c r="A7" s="16"/>
       <c r="B7" s="16"/>
       <c r="C7" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E7" s="81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F7" s="16"/>
       <c r="G7" s="81" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="H7" s="81" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="I7" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J7" s="63" t="str">
         <f t="shared" si="0"/>
@@ -27072,23 +26782,23 @@
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="81" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E8" s="81" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F8" s="16"/>
       <c r="G8" s="81" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="H8" s="81" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="I8" s="81" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J8" s="63" t="str">
         <f t="shared" si="0"/>
@@ -30293,7 +30003,7 @@
   <sheetData>
     <row r="1" spans="1:31" ht="18" customHeight="1">
       <c r="A1" s="85" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="83"/>
       <c r="C1" s="83"/>
@@ -30308,37 +30018,37 @@
     </row>
     <row r="2" spans="1:31" ht="15" customHeight="1">
       <c r="A2" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="67" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="67" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="68" t="s">
+      <c r="D2" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="68" t="s">
+      <c r="E2" s="68" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="68" t="s">
+      <c r="F2" s="41" t="s">
         <v>59</v>
-      </c>
-      <c r="F2" s="41" t="s">
-        <v>60</v>
       </c>
       <c r="G2" s="41" t="s">
         <v>34</v>
       </c>
       <c r="H2" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="I2" s="68" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="68" t="s">
+      <c r="J2" s="68" t="s">
         <v>62</v>
       </c>
-      <c r="J2" s="68" t="s">
+      <c r="K2" s="68" t="s">
         <v>63</v>
-      </c>
-      <c r="K2" s="68" t="s">
-        <v>64</v>
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="41"/>
@@ -35778,27 +35488,27 @@
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" customHeight="1">
       <c r="A1" s="79" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="40.5" customHeight="1">
       <c r="A2" s="80" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="40.5" customHeight="1">
       <c r="A3" s="80" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="40.5" customHeight="1">
       <c r="A4" s="80" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="40.5" customHeight="1">
       <c r="A5" s="80" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="22.5" customHeight="1">
@@ -35806,7 +35516,7 @@
     </row>
     <row r="7" spans="1:1" ht="22.5" customHeight="1">
       <c r="A7" s="80" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="22.5" customHeight="1">

</xml_diff>

<commit_message>
standardized naming of all compile functions and their outputs
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="539" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="309">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -1124,6 +1124,162 @@
   <si>
     <t>https://drive.google.com/file/d/1bfUF7zDY_TFipiMsfsvGmBwkxd0qMgSn/export?format=pdf</t>
   </si>
+  <si>
+    <t>1w_rLdq_TAef4e2Ge83j3NCGZqdYtDMclK67xgQdR2jw</t>
+  </si>
+  <si>
+    <t>13KfMPEbmaXnN4--QVol3liGXUi7Saas46gnm4Qz5rto</t>
+  </si>
+  <si>
+    <t>1oGcH9nQZnII-5SyKuSZ3wz4IEXZTMQ6FNMF7yTWGz0Y</t>
+  </si>
+  <si>
+    <t>1ZD9CBPZDe3cJpn7jC_uWJG--WYz8O1heJE0z3pYzgbU</t>
+  </si>
+  <si>
+    <t>1Kpou_F9LW4aWcRWJUEZ7Gc_ohNDPTgN7u1FcofTGBq8</t>
+  </si>
+  <si>
+    <t>trashed?</t>
+  </si>
+  <si>
+    <t>Fri May 14 14:11:01 2021</t>
+  </si>
+  <si>
+    <t>1-xkENqDwXLz62_UHXWAmQ2eJPCUpNywXB-uz1dywIak</t>
+  </si>
+  <si>
+    <t>1s3lfQ-UHWqrUq4rd1EQg_BjhjAKkG4SJavR7_EKR3Sw</t>
+  </si>
+  <si>
+    <t>1AYdI3aj9WQdFl_eCPDXpnlwMc13pwmNsxnwdM1sZ9iM</t>
+  </si>
+  <si>
+    <t>1vyCDH9FccecJV0umctV--9nWmdKikbVQ47ToKUtYq8Y</t>
+  </si>
+  <si>
+    <t>1eIAjDroQeOw49kK0WSf0CP0I_Jz-AJtKt8hlSDt4m84</t>
+  </si>
+  <si>
+    <t>1W5QIqGEzFLbRKzk9wvvO0rVhCt3t5Fa0sDaK6i9btto</t>
+  </si>
+  <si>
+    <t>1LwYzfh-fwMu8Ej3Pn_0A0Cul3LSTQy8tcX1YWA3WjYo</t>
+  </si>
+  <si>
+    <t>1y5C2w1bJouuCE-_T383eDUKXREfU3OblxYHm10lfVy4</t>
+  </si>
+  <si>
+    <t>1xLtmCyK5PpRS3JsB-TFmQUYdM-AiQkzg_dmNF7ZTisc</t>
+  </si>
+  <si>
+    <t>16f_VJ2xCNy2qzs4majLlMbVDzf93pYYXTkKmcqwr9kc</t>
+  </si>
+  <si>
+    <t>1vnBk3WbFTuQ5wzrBw6yzyKUlql4PdnDeMmqLcD2Hkk8</t>
+  </si>
+  <si>
+    <t>1IeOvMypCE2OTjMf3ZEe9MmcoF0NB1YzRPTHbl8xaeqU</t>
+  </si>
+  <si>
+    <t>1q6I_M1oTIWb3JxwJ8NDud1ECt248RiqZR6BjkYJLiJ8</t>
+  </si>
+  <si>
+    <t>1oyXAIwwgtQEOpt2W8lvx2iWx1xMRQaXVlITqcnVBjAs</t>
+  </si>
+  <si>
+    <t>1a9PDt1ImC0JG7_vZqh-yXcCa7RYBa-DqyRfbqRDZsVE</t>
+  </si>
+  <si>
+    <t>1XMeydMI5WUk7bajhazvqFjQcS9yUwRSu2-9VVM4H13A</t>
+  </si>
+  <si>
+    <t>1ccHAO3mwI59t38HbyyCYEyKrrPGjO9rljQojC9vFmic</t>
+  </si>
+  <si>
+    <t>1yBey9NeTjqDxBEEv-7hlJjDtIse3bkB_X8JCbxhGPqA</t>
+  </si>
+  <si>
+    <t>1hDWushBDAAwUuEuUdr--hGqrMyUriHnw9Y41zOMHHC0</t>
+  </si>
+  <si>
+    <t>10uU0I3GL-rUIIfcIw5gVeO9A1A3rwX1W2-x1wApwdPI</t>
+  </si>
+  <si>
+    <t>1U2jpqM1ipy0h-L_001kItL93AfXT6AQtj9P3YoEdfI0</t>
+  </si>
+  <si>
+    <t>1L737p4jTBB4XCd_hfzDm7xQqEt3nRosBk67yTjqQReE</t>
+  </si>
+  <si>
+    <t>1s2qYrx_88xEfeRNM530Jxs4cLbJeRPzmfI7cd7UQDT8</t>
+  </si>
+  <si>
+    <t>1zeTb9Y37V6hZ1DxH5LGXD0bnqCI5zQHj5-fFlqxRgqg</t>
+  </si>
+  <si>
+    <t>192-nPS5k_nTkyQw7FrXEZ0jwerqWoXRmYNcwqiuEeJc</t>
+  </si>
+  <si>
+    <t>1-CIgtCumwSnOnMVpq8t-Izxro48D76i-DyLH7z-qAQc</t>
+  </si>
+  <si>
+    <t>1AERHj7Jx8o7vcG1Ejza-fsyYBIU3oSv4oyhT-dcaUTU</t>
+  </si>
+  <si>
+    <t>1OU81GWUHonBjilSnjr390gGIzZUHhEh_CWVxx_-4SfQ</t>
+  </si>
+  <si>
+    <t>1w7aK0dBglK5NedpIMWnx9Cz0Xwfg7U1MQqPVDEc1kxg</t>
+  </si>
+  <si>
+    <t>1f4-nC_VBrKdLCU6gHucbTkByVheTHtE668OXqNpzdME</t>
+  </si>
+  <si>
+    <t>1jYxTsIVv8skH_MvGCjLa9YtDl4WEGMi_1a079sbMtAE</t>
+  </si>
+  <si>
+    <t>1a0dRiYA_L0LG_4KE6dImmgGQHkZtG4utPvn816DoXOw</t>
+  </si>
+  <si>
+    <t>1DfeLRvKqv1pAmX3tIuEkaYcd1elWOk0pJ9ipldRCYtY</t>
+  </si>
+  <si>
+    <t>1D6o1ybWAXYUob4o0rQiDfmOYRf0S0sMhkXBR3zgUlyA</t>
+  </si>
+  <si>
+    <t>1JvfwHaXqbsv6HN9gJAQI4AuAKKHKvza89mqHPqJ3GO8</t>
+  </si>
+  <si>
+    <t>1Tcp52KncP2JGJK5YOgKq-CgCTR4UjsFyXHbYnz86WvU</t>
+  </si>
+  <si>
+    <t>1ZS2e0Y8s74Fq85ak4OOi7_VLEcGQpCKpP5koCG1V5e8</t>
+  </si>
+  <si>
+    <t>1OpS9bS983mfrnL8IqBST0FhsNMUVrRQfWGsE8L0Xq1g</t>
+  </si>
+  <si>
+    <t>1YYFWZVN7u0fPKAiJ5irMieGN6h0-uuAvQKsasp1r5ss</t>
+  </si>
+  <si>
+    <t>1bYbtq5DOUW6u7BJAlG4-UZZ8fhkuuQjg</t>
+  </si>
+  <si>
+    <t>1bn-_Hgkuqdtjq4o7aOeOC_XtydBRSfXK</t>
+  </si>
+  <si>
+    <t>1bRfT56hbO6uOeOBqzr5U-gI_pte2X7Pd</t>
+  </si>
+  <si>
+    <t>1blBvoHgc0slnpmVIuL24GTqSQfwOyFmH</t>
+  </si>
+  <si>
+    <t>1bC4McsjvWeBLTnfedsL7GxytaFy60NFF</t>
+  </si>
+  <si>
+    <t>1bfUF7zDY_TFipiMsfsvGmBwkxd0qMgSn</t>
+  </si>
 </sst>
 </file>
 
@@ -1557,7 +1713,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="605">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1709,6 +1865,1518 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2023,12 +3691,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="21.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="29.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="27.33203125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="8.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="25.6640625" collapsed="false"/>
-    <col min="6" max="26" customWidth="true" width="10.6640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="6" max="26" customWidth="true" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="18" customHeight="1">
@@ -9498,16 +11166,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.83203125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="16.5" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="8.5" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="11.1640625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="15.5" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="21.6640625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="75" width="21.5" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" style="75" width="38.83203125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="21.6640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="75" width="21.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" style="75" width="38.83203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="21.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="21" customHeight="1">
@@ -9574,115 +11242,125 @@
     </row>
     <row r="3" spans="1:29" ht="28.5" customHeight="1">
       <c r="A3" s="12"/>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="101" t="s">
         <v>73</v>
       </c>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="109" t="s">
         <v>79</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="114" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="119" t="s">
         <v>89</v>
       </c>
       <c r="G3" s="15"/>
-      <c r="H3" s="97" t="s">
+      <c r="H3" s="124" t="s">
         <v>90</v>
       </c>
       <c r="I3" s="76"/>
-      <c r="J3"/>
+      <c r="J3" t="s" s="127">
+        <v>257</v>
+      </c>
     </row>
     <row r="4" spans="1:29" ht="28.5" customHeight="1">
       <c r="A4" s="12"/>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="102" t="s">
         <v>74</v>
       </c>
       <c r="C4" s="12"/>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="110" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="115" t="s">
         <v>85</v>
       </c>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="120" t="s">
         <v>89</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="74"/>
       <c r="I4" s="76"/>
-      <c r="J4"/>
+      <c r="J4" t="s" s="128">
+        <v>258</v>
+      </c>
     </row>
     <row r="5" spans="1:29" ht="28.5" customHeight="1">
       <c r="A5" s="12"/>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="103" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="107" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="111" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="116" t="s">
         <v>86</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="121" t="s">
         <v>89</v>
       </c>
       <c r="G5" s="15"/>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="125" t="s">
         <v>91</v>
       </c>
       <c r="I5" s="76"/>
-      <c r="J5"/>
+      <c r="J5" t="s" s="129">
+        <v>259</v>
+      </c>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1">
       <c r="A6" s="12"/>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="104" t="s">
         <v>73</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="112" t="s">
         <v>82</v>
       </c>
-      <c r="E6" s="97" t="s">
+      <c r="E6" s="117" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="122" t="s">
         <v>89</v>
       </c>
       <c r="G6" s="15"/>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="126" t="s">
         <v>92</v>
       </c>
       <c r="I6" s="76"/>
-      <c r="J6"/>
+      <c r="J6" t="s" s="130">
+        <v>260</v>
+      </c>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1">
       <c r="A7" s="12"/>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="105" t="s">
         <v>75</v>
       </c>
       <c r="C7" s="16"/>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="113" t="s">
         <v>83</v>
       </c>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="118" t="s">
         <v>88</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="123" t="s">
         <v>89</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="74"/>
       <c r="I7" s="76"/>
-      <c r="J7"/>
+      <c r="J7" t="s" s="131">
+        <v>261</v>
+      </c>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1">
       <c r="A8" s="12"/>
@@ -11022,13 +12700,13 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.33203125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.6640625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="22.83203125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="21.6640625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="112.5" collapsed="false"/>
-    <col min="7" max="27" customWidth="true" width="10.6640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="22.83203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="112.5" collapsed="true"/>
+    <col min="7" max="27" customWidth="true" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="19.5" customHeight="1">
@@ -11083,25 +12761,27 @@
       <c r="AA2" s="4"/>
     </row>
     <row r="3" spans="1:27" ht="18" customHeight="1">
-      <c r="A3" s="97" t="s">
+      <c r="A3" s="132" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="148" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="164" t="s">
         <v>93</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="180" t="s">
         <v>97</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="196" t="s">
         <v>105</v>
       </c>
-      <c r="F3" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="G3" s="17"/>
+      <c r="F3" s="212" t="s">
+        <v>262</v>
+      </c>
+      <c r="G3" s="228" t="s">
+        <v>105</v>
+      </c>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -11115,25 +12795,27 @@
       <c r="R3" s="17"/>
     </row>
     <row r="4" spans="1:27" ht="18" customHeight="1">
-      <c r="A4" s="97" t="s">
+      <c r="A4" s="133" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="97" t="s">
+      <c r="B4" s="149" t="s">
         <v>94</v>
       </c>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="165" t="s">
         <v>93</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="181" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="197" t="s">
         <v>106</v>
       </c>
-      <c r="F4" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" s="17"/>
+      <c r="F4" s="213" t="s">
+        <v>262</v>
+      </c>
+      <c r="G4" s="229" t="s">
+        <v>106</v>
+      </c>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
@@ -11147,25 +12829,27 @@
       <c r="R4" s="17"/>
     </row>
     <row r="5" spans="1:27" ht="18" customHeight="1">
-      <c r="A5" s="97" t="s">
+      <c r="A5" s="134" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="97" t="s">
+      <c r="B5" s="150" t="s">
         <v>95</v>
       </c>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="166" t="s">
         <v>93</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="182" t="s">
         <v>99</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="198" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="G5" s="17"/>
+      <c r="F5" s="214" t="s">
+        <v>262</v>
+      </c>
+      <c r="G5" s="230" t="s">
+        <v>107</v>
+      </c>
       <c r="H5" s="17"/>
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
@@ -11179,25 +12863,27 @@
       <c r="R5" s="17"/>
     </row>
     <row r="6" spans="1:27" ht="18" customHeight="1">
-      <c r="A6" s="97" t="s">
+      <c r="A6" s="135" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="151" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="167" t="s">
         <v>93</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="183" t="s">
         <v>100</v>
       </c>
-      <c r="E6" s="97" t="s">
+      <c r="E6" s="199" t="s">
         <v>108</v>
       </c>
-      <c r="F6" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="G6" s="17"/>
+      <c r="F6" s="215" t="s">
+        <v>262</v>
+      </c>
+      <c r="G6" s="231" t="s">
+        <v>108</v>
+      </c>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -11211,25 +12897,27 @@
       <c r="R6" s="17"/>
     </row>
     <row r="7" spans="1:27" ht="18" customHeight="1">
-      <c r="A7" s="97" t="s">
+      <c r="A7" s="136" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="97" t="s">
+      <c r="B7" s="152" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="97" t="s">
+      <c r="C7" s="168" t="s">
         <v>93</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="184" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="200" t="s">
         <v>109</v>
       </c>
-      <c r="F7" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="G7" s="17"/>
+      <c r="F7" s="216" t="s">
+        <v>262</v>
+      </c>
+      <c r="G7" s="232" t="s">
+        <v>109</v>
+      </c>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
@@ -11243,25 +12931,27 @@
       <c r="R7" s="17"/>
     </row>
     <row r="8" spans="1:27" ht="18" customHeight="1">
-      <c r="A8" s="97" t="s">
+      <c r="A8" s="137" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="97" t="s">
+      <c r="B8" s="153" t="s">
         <v>96</v>
       </c>
-      <c r="C8" s="97" t="s">
+      <c r="C8" s="169" t="s">
         <v>93</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="185" t="s">
         <v>102</v>
       </c>
-      <c r="E8" s="97" t="s">
+      <c r="E8" s="201" t="s">
         <v>110</v>
       </c>
-      <c r="F8" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="G8" s="17"/>
+      <c r="F8" s="217" t="s">
+        <v>262</v>
+      </c>
+      <c r="G8" s="233" t="s">
+        <v>110</v>
+      </c>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
       <c r="J8" s="17"/>
@@ -11275,25 +12965,27 @@
       <c r="R8" s="17"/>
     </row>
     <row r="9" spans="1:27" ht="18" customHeight="1">
-      <c r="A9" s="97" t="s">
+      <c r="A9" s="138" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="154" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="97" t="s">
+      <c r="C9" s="170" t="s">
         <v>93</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="186" t="s">
         <v>103</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="202" t="s">
         <v>111</v>
       </c>
-      <c r="F9" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="G9" s="17"/>
+      <c r="F9" s="218" t="s">
+        <v>262</v>
+      </c>
+      <c r="G9" s="234" t="s">
+        <v>111</v>
+      </c>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
@@ -11307,25 +12999,27 @@
       <c r="R9" s="17"/>
     </row>
     <row r="10" spans="1:27" ht="18" customHeight="1">
-      <c r="A10" s="97" t="s">
+      <c r="A10" s="139" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="97" t="s">
+      <c r="B10" s="155" t="s">
         <v>94</v>
       </c>
-      <c r="C10" s="97" t="s">
+      <c r="C10" s="171" t="s">
         <v>93</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="187" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="97" t="s">
+      <c r="E10" s="203" t="s">
         <v>112</v>
       </c>
-      <c r="F10" s="97" t="s">
-        <v>89</v>
-      </c>
-      <c r="G10" s="17"/>
+      <c r="F10" s="219" t="s">
+        <v>262</v>
+      </c>
+      <c r="G10" s="235" t="s">
+        <v>112</v>
+      </c>
       <c r="H10" s="17"/>
       <c r="I10" s="17"/>
       <c r="J10" s="17"/>
@@ -11339,12 +13033,24 @@
       <c r="R10" s="17"/>
     </row>
     <row r="11" spans="1:27" ht="18" customHeight="1">
-      <c r="A11" s="5"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="16"/>
+      <c r="A11" s="140" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="156" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="172" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="188" t="s">
+        <v>97</v>
+      </c>
+      <c r="E11" s="204" t="s">
+        <v>105</v>
+      </c>
+      <c r="F11" s="220" t="s">
+        <v>263</v>
+      </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
@@ -11359,12 +13065,24 @@
       <c r="R11" s="17"/>
     </row>
     <row r="12" spans="1:27" ht="18" customHeight="1">
-      <c r="A12" s="5"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="16"/>
+      <c r="A12" s="141" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="157" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="173" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="189" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="205" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="221" t="s">
+        <v>263</v>
+      </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -11379,12 +13097,24 @@
       <c r="R12" s="17"/>
     </row>
     <row r="13" spans="1:27" ht="18" customHeight="1">
-      <c r="A13" s="5"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="16"/>
+      <c r="A13" s="142" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="158" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="174" t="s">
+        <v>93</v>
+      </c>
+      <c r="D13" s="190" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="206" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="222" t="s">
+        <v>263</v>
+      </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
@@ -11399,12 +13129,24 @@
       <c r="R13" s="17"/>
     </row>
     <row r="14" spans="1:27" ht="18" customHeight="1">
-      <c r="A14" s="5"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="16"/>
+      <c r="A14" s="143" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="159" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="175" t="s">
+        <v>93</v>
+      </c>
+      <c r="D14" s="191" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="207" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="223" t="s">
+        <v>263</v>
+      </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
       <c r="I14" s="17"/>
@@ -11419,12 +13161,24 @@
       <c r="R14" s="17"/>
     </row>
     <row r="15" spans="1:27" ht="18" customHeight="1">
-      <c r="A15" s="5"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="16"/>
+      <c r="A15" s="144" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="160" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="176" t="s">
+        <v>93</v>
+      </c>
+      <c r="D15" s="192" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="208" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="224" t="s">
+        <v>263</v>
+      </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
       <c r="I15" s="17"/>
@@ -11439,12 +13193,24 @@
       <c r="R15" s="17"/>
     </row>
     <row r="16" spans="1:27" ht="18" customHeight="1">
-      <c r="A16" s="5"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="16"/>
+      <c r="A16" s="145" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="161" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" s="177" t="s">
+        <v>93</v>
+      </c>
+      <c r="D16" s="193" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="209" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="225" t="s">
+        <v>263</v>
+      </c>
       <c r="G16" s="17"/>
       <c r="H16" s="17"/>
       <c r="I16" s="17"/>
@@ -11459,12 +13225,24 @@
       <c r="R16" s="17"/>
     </row>
     <row r="17" spans="1:18" ht="18" customHeight="1">
-      <c r="A17" s="5"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
-      <c r="F17" s="16"/>
+      <c r="A17" s="146" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="162" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17" s="194" t="s">
+        <v>103</v>
+      </c>
+      <c r="E17" s="210" t="s">
+        <v>111</v>
+      </c>
+      <c r="F17" s="226" t="s">
+        <v>263</v>
+      </c>
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="17"/>
@@ -11479,12 +13257,24 @@
       <c r="R17" s="17"/>
     </row>
     <row r="18" spans="1:18" ht="18" customHeight="1">
-      <c r="A18" s="5"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
-      <c r="F18" s="16"/>
+      <c r="A18" s="147" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" s="163" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="179" t="s">
+        <v>93</v>
+      </c>
+      <c r="D18" s="195" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18" s="211" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="227" t="s">
+        <v>263</v>
+      </c>
       <c r="G18" s="17"/>
       <c r="H18" s="17"/>
       <c r="I18" s="17"/>
@@ -18639,17 +20429,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="9.6640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.5" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.5" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="8.5" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="28.5" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.5" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="8" max="9" customWidth="true" style="75" width="21.5" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="75" width="35.1640625" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="16.6640625" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="21.6640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="28.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="8" max="9" customWidth="true" style="75" width="21.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="75" width="35.1640625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="21.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="19.5" customHeight="1">
@@ -18725,253 +20515,271 @@
     <row r="3" spans="1:32" ht="17">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="236" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="245" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="254" t="s">
         <v>113</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="263" t="s">
         <v>122</v>
       </c>
-      <c r="G3" s="97" t="s">
+      <c r="G3" s="272" t="s">
         <v>89</v>
       </c>
-      <c r="H3" s="97" t="s">
+      <c r="H3" s="281" t="s">
         <v>131</v>
       </c>
-      <c r="I3" s="97" t="s">
+      <c r="I3" s="290" t="s">
         <v>140</v>
       </c>
       <c r="J3" s="76"/>
-      <c r="K3" s="26"/>
+      <c r="K3" s="299" t="s">
+        <v>264</v>
+      </c>
       <c r="L3" s="27"/>
     </row>
     <row r="4" spans="1:32" ht="17">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="237" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="246" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="255" t="s">
         <v>114</v>
       </c>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="264" t="s">
         <v>123</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="273" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="282" t="s">
         <v>132</v>
       </c>
-      <c r="I4" s="97" t="s">
+      <c r="I4" s="291" t="s">
         <v>141</v>
       </c>
       <c r="J4" s="76"/>
-      <c r="K4" s="26"/>
+      <c r="K4" s="300" t="s">
+        <v>265</v>
+      </c>
       <c r="L4" s="27"/>
     </row>
     <row r="5" spans="1:32" ht="17">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="238" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="247" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="256" t="s">
         <v>115</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="265" t="s">
         <v>124</v>
       </c>
-      <c r="G5" s="97" t="s">
+      <c r="G5" s="274" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="283" t="s">
         <v>133</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="292" t="s">
         <v>142</v>
       </c>
       <c r="J5" s="76"/>
-      <c r="K5" s="26"/>
+      <c r="K5" s="301" t="s">
+        <v>266</v>
+      </c>
       <c r="L5" s="27"/>
     </row>
     <row r="6" spans="1:32" ht="17">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="239" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="248" t="s">
         <v>77</v>
       </c>
-      <c r="E6" s="97" t="s">
+      <c r="E6" s="257" t="s">
         <v>116</v>
       </c>
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="266" t="s">
         <v>125</v>
       </c>
-      <c r="G6" s="97" t="s">
+      <c r="G6" s="275" t="s">
         <v>89</v>
       </c>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="284" t="s">
         <v>134</v>
       </c>
-      <c r="I6" s="97" t="s">
+      <c r="I6" s="293" t="s">
         <v>143</v>
       </c>
       <c r="J6" s="76"/>
-      <c r="K6" s="26"/>
+      <c r="K6" s="302" t="s">
+        <v>267</v>
+      </c>
       <c r="L6" s="27"/>
     </row>
     <row r="7" spans="1:32" ht="17">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="97" t="s">
+      <c r="C7" s="240" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="249" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="258" t="s">
         <v>117</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="267" t="s">
         <v>126</v>
       </c>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="276" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="97" t="s">
+      <c r="H7" s="285" t="s">
         <v>135</v>
       </c>
-      <c r="I7" s="97" t="s">
+      <c r="I7" s="294" t="s">
         <v>144</v>
       </c>
       <c r="J7" s="76"/>
-      <c r="K7" s="26"/>
+      <c r="K7" s="303" t="s">
+        <v>268</v>
+      </c>
       <c r="L7" s="27"/>
     </row>
     <row r="8" spans="1:32" ht="17">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="97" t="s">
+      <c r="C8" s="241" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="250" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="97" t="s">
+      <c r="E8" s="259" t="s">
         <v>118</v>
       </c>
-      <c r="F8" s="97" t="s">
+      <c r="F8" s="268" t="s">
         <v>127</v>
       </c>
-      <c r="G8" s="97" t="s">
+      <c r="G8" s="277" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="97" t="s">
+      <c r="H8" s="286" t="s">
         <v>136</v>
       </c>
-      <c r="I8" s="97" t="s">
+      <c r="I8" s="295" t="s">
         <v>145</v>
       </c>
       <c r="J8" s="76"/>
-      <c r="K8" s="26"/>
+      <c r="K8" s="304" t="s">
+        <v>269</v>
+      </c>
       <c r="L8" s="27"/>
     </row>
     <row r="9" spans="1:32" ht="17">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="97" t="s">
+      <c r="C9" s="242" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="251" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="260" t="s">
         <v>119</v>
       </c>
-      <c r="F9" s="97" t="s">
+      <c r="F9" s="269" t="s">
         <v>128</v>
       </c>
-      <c r="G9" s="97" t="s">
+      <c r="G9" s="278" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="97" t="s">
+      <c r="H9" s="287" t="s">
         <v>137</v>
       </c>
-      <c r="I9" s="97" t="s">
+      <c r="I9" s="296" t="s">
         <v>146</v>
       </c>
       <c r="J9" s="76"/>
-      <c r="K9" s="26"/>
+      <c r="K9" s="305" t="s">
+        <v>270</v>
+      </c>
       <c r="L9" s="27"/>
     </row>
     <row r="10" spans="1:32" ht="17">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="97" t="s">
+      <c r="C10" s="243" t="s">
         <v>96</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="252" t="s">
         <v>77</v>
       </c>
-      <c r="E10" s="97" t="s">
+      <c r="E10" s="261" t="s">
         <v>120</v>
       </c>
-      <c r="F10" s="97" t="s">
+      <c r="F10" s="270" t="s">
         <v>129</v>
       </c>
-      <c r="G10" s="97" t="s">
+      <c r="G10" s="279" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="97" t="s">
+      <c r="H10" s="288" t="s">
         <v>138</v>
       </c>
-      <c r="I10" s="97" t="s">
+      <c r="I10" s="297" t="s">
         <v>147</v>
       </c>
       <c r="J10" s="76"/>
-      <c r="K10" s="26"/>
+      <c r="K10" s="306" t="s">
+        <v>271</v>
+      </c>
       <c r="L10" s="27"/>
     </row>
     <row r="11" spans="1:32" ht="17">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="244" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="97" t="s">
+      <c r="D11" s="253" t="s">
         <v>76</v>
       </c>
-      <c r="E11" s="97" t="s">
+      <c r="E11" s="262" t="s">
         <v>121</v>
       </c>
-      <c r="F11" s="97" t="s">
+      <c r="F11" s="271" t="s">
         <v>130</v>
       </c>
-      <c r="G11" s="97" t="s">
+      <c r="G11" s="280" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="97" t="s">
+      <c r="H11" s="289" t="s">
         <v>139</v>
       </c>
-      <c r="I11" s="97" t="s">
+      <c r="I11" s="298" t="s">
         <v>148</v>
       </c>
       <c r="J11" s="76"/>
-      <c r="K11" s="26"/>
+      <c r="K11" s="307" t="s">
+        <v>272</v>
+      </c>
       <c r="L11" s="27"/>
     </row>
     <row r="12" spans="1:32" ht="15.75" customHeight="1">
@@ -20785,18 +22593,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.1640625" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="11.6640625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.5" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="9.5" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="10.5" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.83203125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="29.6640625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="16.5" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="19.1640625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="75" width="21.5" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" style="75" width="19.0" collapsed="false"/>
-    <col min="12" max="31" customWidth="true" width="10.6640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.1640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.83203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="29.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.1640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="75" width="21.5" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" style="75" width="19.0" collapsed="true"/>
+    <col min="12" max="31" customWidth="true" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="19.5" customHeight="1">
@@ -20892,32 +22700,34 @@
     <row r="3" spans="1:31" ht="18">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="308" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="329" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="350" t="s">
         <v>149</v>
       </c>
       <c r="F3" s="12"/>
-      <c r="G3" s="97" t="s">
+      <c r="G3" s="368" t="s">
         <v>151</v>
       </c>
-      <c r="H3" s="97" t="s">
+      <c r="H3" s="389" t="s">
         <v>172</v>
       </c>
-      <c r="I3" s="97" t="s">
+      <c r="I3" s="410" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="97" t="s">
+      <c r="J3" s="431" t="s">
         <v>193</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="K3" s="452" t="s">
         <v>193</v>
       </c>
-      <c r="L3" s="6"/>
+      <c r="L3" s="473" t="s">
+        <v>273</v>
+      </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -20937,32 +22747,34 @@
     <row r="4" spans="1:31" ht="18">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="309" t="s">
         <v>94</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="330" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="351" t="s">
         <v>150</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="369" t="s">
         <v>152</v>
       </c>
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="390" t="s">
         <v>173</v>
       </c>
-      <c r="I4" s="97" t="s">
+      <c r="I4" s="411" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="97" t="s">
+      <c r="J4" s="432" t="s">
         <v>194</v>
       </c>
-      <c r="K4" s="97" t="s">
+      <c r="K4" s="453" t="s">
         <v>194</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="474" t="s">
+        <v>274</v>
+      </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -20982,32 +22794,34 @@
     <row r="5" spans="1:31" ht="18">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="310" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="331" t="s">
         <v>77</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="352" t="s">
         <v>149</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="97" t="s">
+      <c r="G5" s="370" t="s">
         <v>153</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="391" t="s">
         <v>174</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="412" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="433" t="s">
         <v>195</v>
       </c>
-      <c r="K5" s="97" t="s">
+      <c r="K5" s="454" t="s">
         <v>195</v>
       </c>
-      <c r="L5" s="6"/>
+      <c r="L5" s="475" t="s">
+        <v>275</v>
+      </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
@@ -21027,30 +22841,32 @@
     <row r="6" spans="1:31" ht="18">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="311" t="s">
         <v>94</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="332" t="s">
         <v>78</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
-      <c r="G6" s="97" t="s">
+      <c r="G6" s="371" t="s">
         <v>154</v>
       </c>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="392" t="s">
         <v>175</v>
       </c>
-      <c r="I6" s="97" t="s">
+      <c r="I6" s="413" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="97" t="s">
+      <c r="J6" s="434" t="s">
         <v>196</v>
       </c>
-      <c r="K6" s="97" t="s">
+      <c r="K6" s="455" t="s">
         <v>196</v>
       </c>
-      <c r="L6" s="6"/>
+      <c r="L6" s="476" t="s">
+        <v>276</v>
+      </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -21070,32 +22886,34 @@
     <row r="7" spans="1:31" ht="18">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="97" t="s">
+      <c r="C7" s="312" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="333" t="s">
         <v>76</v>
       </c>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="353" t="s">
         <v>150</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="372" t="s">
         <v>155</v>
       </c>
-      <c r="H7" s="97" t="s">
+      <c r="H7" s="393" t="s">
         <v>176</v>
       </c>
-      <c r="I7" s="97" t="s">
+      <c r="I7" s="414" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="97" t="s">
+      <c r="J7" s="435" t="s">
         <v>197</v>
       </c>
-      <c r="K7" s="97" t="s">
+      <c r="K7" s="456" t="s">
         <v>197</v>
       </c>
-      <c r="L7" s="6"/>
+      <c r="L7" s="477" t="s">
+        <v>277</v>
+      </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -21115,32 +22933,34 @@
     <row r="8" spans="1:31" ht="18">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="97" t="s">
+      <c r="C8" s="313" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="334" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="97" t="s">
+      <c r="E8" s="354" t="s">
         <v>149</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="97" t="s">
+      <c r="G8" s="373" t="s">
         <v>156</v>
       </c>
-      <c r="H8" s="97" t="s">
+      <c r="H8" s="394" t="s">
         <v>177</v>
       </c>
-      <c r="I8" s="97" t="s">
+      <c r="I8" s="415" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="97" t="s">
+      <c r="J8" s="436" t="s">
         <v>198</v>
       </c>
-      <c r="K8" s="97" t="s">
+      <c r="K8" s="457" t="s">
         <v>198</v>
       </c>
-      <c r="L8" s="6"/>
+      <c r="L8" s="478" t="s">
+        <v>278</v>
+      </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -21160,32 +22980,34 @@
     <row r="9" spans="1:31" ht="18">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="97" t="s">
+      <c r="C9" s="314" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="335" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="355" t="s">
         <v>150</v>
       </c>
       <c r="F9" s="12"/>
-      <c r="G9" s="97" t="s">
+      <c r="G9" s="374" t="s">
         <v>157</v>
       </c>
-      <c r="H9" s="97" t="s">
+      <c r="H9" s="395" t="s">
         <v>178</v>
       </c>
-      <c r="I9" s="97" t="s">
+      <c r="I9" s="416" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="97" t="s">
+      <c r="J9" s="437" t="s">
         <v>199</v>
       </c>
-      <c r="K9" s="97" t="s">
+      <c r="K9" s="458" t="s">
         <v>199</v>
       </c>
-      <c r="L9" s="6"/>
+      <c r="L9" s="479" t="s">
+        <v>279</v>
+      </c>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -21205,32 +23027,34 @@
     <row r="10" spans="1:31" ht="18">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="97" t="s">
+      <c r="C10" s="315" t="s">
         <v>95</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="336" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="97" t="s">
+      <c r="E10" s="356" t="s">
         <v>149</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="97" t="s">
+      <c r="G10" s="375" t="s">
         <v>158</v>
       </c>
-      <c r="H10" s="97" t="s">
+      <c r="H10" s="396" t="s">
         <v>179</v>
       </c>
-      <c r="I10" s="97" t="s">
+      <c r="I10" s="417" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="97" t="s">
+      <c r="J10" s="438" t="s">
         <v>200</v>
       </c>
-      <c r="K10" s="97" t="s">
+      <c r="K10" s="459" t="s">
         <v>200</v>
       </c>
-      <c r="L10" s="6"/>
+      <c r="L10" s="480" t="s">
+        <v>280</v>
+      </c>
       <c r="M10" s="6"/>
       <c r="N10" s="6"/>
       <c r="O10" s="6"/>
@@ -21250,32 +23074,34 @@
     <row r="11" spans="1:31" ht="18">
       <c r="A11" s="12"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="316" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="97" t="s">
+      <c r="D11" s="337" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="97" t="s">
+      <c r="E11" s="357" t="s">
         <v>150</v>
       </c>
       <c r="F11" s="12"/>
-      <c r="G11" s="97" t="s">
+      <c r="G11" s="376" t="s">
         <v>159</v>
       </c>
-      <c r="H11" s="97" t="s">
+      <c r="H11" s="397" t="s">
         <v>180</v>
       </c>
-      <c r="I11" s="97" t="s">
+      <c r="I11" s="418" t="s">
         <v>89</v>
       </c>
-      <c r="J11" s="97" t="s">
+      <c r="J11" s="439" t="s">
         <v>201</v>
       </c>
-      <c r="K11" s="97" t="s">
+      <c r="K11" s="460" t="s">
         <v>201</v>
       </c>
-      <c r="L11" s="6"/>
+      <c r="L11" s="481" t="s">
+        <v>281</v>
+      </c>
       <c r="M11" s="6"/>
       <c r="N11" s="6"/>
       <c r="O11" s="6"/>
@@ -21295,32 +23121,34 @@
     <row r="12" spans="1:31" ht="18">
       <c r="A12" s="12"/>
       <c r="B12" s="12"/>
-      <c r="C12" s="97" t="s">
+      <c r="C12" s="317" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="97" t="s">
+      <c r="D12" s="338" t="s">
         <v>77</v>
       </c>
-      <c r="E12" s="97" t="s">
+      <c r="E12" s="358" t="s">
         <v>149</v>
       </c>
       <c r="F12" s="12"/>
-      <c r="G12" s="97" t="s">
+      <c r="G12" s="377" t="s">
         <v>160</v>
       </c>
-      <c r="H12" s="97" t="s">
+      <c r="H12" s="398" t="s">
         <v>181</v>
       </c>
-      <c r="I12" s="97" t="s">
+      <c r="I12" s="419" t="s">
         <v>89</v>
       </c>
-      <c r="J12" s="97" t="s">
+      <c r="J12" s="440" t="s">
         <v>202</v>
       </c>
-      <c r="K12" s="97" t="s">
+      <c r="K12" s="461" t="s">
         <v>202</v>
       </c>
-      <c r="L12" s="6"/>
+      <c r="L12" s="482" t="s">
+        <v>282</v>
+      </c>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
@@ -21340,30 +23168,32 @@
     <row r="13" spans="1:31" ht="18">
       <c r="A13" s="12"/>
       <c r="B13" s="12"/>
-      <c r="C13" s="97" t="s">
+      <c r="C13" s="318" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="97" t="s">
+      <c r="D13" s="339" t="s">
         <v>78</v>
       </c>
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
-      <c r="G13" s="97" t="s">
+      <c r="G13" s="378" t="s">
         <v>161</v>
       </c>
-      <c r="H13" s="97" t="s">
+      <c r="H13" s="399" t="s">
         <v>182</v>
       </c>
-      <c r="I13" s="97" t="s">
+      <c r="I13" s="420" t="s">
         <v>89</v>
       </c>
-      <c r="J13" s="97" t="s">
+      <c r="J13" s="441" t="s">
         <v>203</v>
       </c>
-      <c r="K13" s="97" t="s">
+      <c r="K13" s="462" t="s">
         <v>203</v>
       </c>
-      <c r="L13" s="6"/>
+      <c r="L13" s="483" t="s">
+        <v>283</v>
+      </c>
       <c r="M13" s="6"/>
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
@@ -21383,32 +23213,34 @@
     <row r="14" spans="1:31" ht="18">
       <c r="A14" s="12"/>
       <c r="B14" s="12"/>
-      <c r="C14" s="97" t="s">
+      <c r="C14" s="319" t="s">
         <v>95</v>
       </c>
-      <c r="D14" s="97" t="s">
+      <c r="D14" s="340" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="97" t="s">
+      <c r="E14" s="359" t="s">
         <v>149</v>
       </c>
       <c r="F14" s="12"/>
-      <c r="G14" s="97" t="s">
+      <c r="G14" s="379" t="s">
         <v>162</v>
       </c>
-      <c r="H14" s="97" t="s">
+      <c r="H14" s="400" t="s">
         <v>183</v>
       </c>
-      <c r="I14" s="97" t="s">
+      <c r="I14" s="421" t="s">
         <v>89</v>
       </c>
-      <c r="J14" s="97" t="s">
+      <c r="J14" s="442" t="s">
         <v>204</v>
       </c>
-      <c r="K14" s="97" t="s">
+      <c r="K14" s="463" t="s">
         <v>204</v>
       </c>
-      <c r="L14" s="6"/>
+      <c r="L14" s="484" t="s">
+        <v>284</v>
+      </c>
       <c r="M14" s="6"/>
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
@@ -21428,32 +23260,34 @@
     <row r="15" spans="1:31" ht="18">
       <c r="A15" s="12"/>
       <c r="B15" s="12"/>
-      <c r="C15" s="97" t="s">
+      <c r="C15" s="320" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="97" t="s">
+      <c r="D15" s="341" t="s">
         <v>76</v>
       </c>
-      <c r="E15" s="97" t="s">
+      <c r="E15" s="360" t="s">
         <v>150</v>
       </c>
       <c r="F15" s="12"/>
-      <c r="G15" s="97" t="s">
+      <c r="G15" s="380" t="s">
         <v>163</v>
       </c>
-      <c r="H15" s="97" t="s">
+      <c r="H15" s="401" t="s">
         <v>184</v>
       </c>
-      <c r="I15" s="97" t="s">
+      <c r="I15" s="422" t="s">
         <v>89</v>
       </c>
-      <c r="J15" s="97" t="s">
+      <c r="J15" s="443" t="s">
         <v>205</v>
       </c>
-      <c r="K15" s="97" t="s">
+      <c r="K15" s="464" t="s">
         <v>205</v>
       </c>
-      <c r="L15" s="6"/>
+      <c r="L15" s="485" t="s">
+        <v>285</v>
+      </c>
       <c r="M15" s="6"/>
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
@@ -21473,32 +23307,34 @@
     <row r="16" spans="1:31" ht="18">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
-      <c r="C16" s="97" t="s">
+      <c r="C16" s="321" t="s">
         <v>95</v>
       </c>
-      <c r="D16" s="97" t="s">
+      <c r="D16" s="342" t="s">
         <v>77</v>
       </c>
-      <c r="E16" s="97" t="s">
+      <c r="E16" s="361" t="s">
         <v>150</v>
       </c>
       <c r="F16" s="12"/>
-      <c r="G16" s="97" t="s">
+      <c r="G16" s="381" t="s">
         <v>164</v>
       </c>
-      <c r="H16" s="97" t="s">
+      <c r="H16" s="402" t="s">
         <v>185</v>
       </c>
-      <c r="I16" s="97" t="s">
+      <c r="I16" s="423" t="s">
         <v>89</v>
       </c>
-      <c r="J16" s="97" t="s">
+      <c r="J16" s="444" t="s">
         <v>206</v>
       </c>
-      <c r="K16" s="97" t="s">
+      <c r="K16" s="465" t="s">
         <v>206</v>
       </c>
-      <c r="L16" s="6"/>
+      <c r="L16" s="486" t="s">
+        <v>286</v>
+      </c>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
@@ -21518,30 +23354,32 @@
     <row r="17" spans="1:27" ht="18">
       <c r="A17" s="12"/>
       <c r="B17" s="12"/>
-      <c r="C17" s="97" t="s">
+      <c r="C17" s="322" t="s">
         <v>96</v>
       </c>
-      <c r="D17" s="97" t="s">
+      <c r="D17" s="343" t="s">
         <v>78</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
-      <c r="G17" s="97" t="s">
+      <c r="G17" s="382" t="s">
         <v>165</v>
       </c>
-      <c r="H17" s="97" t="s">
+      <c r="H17" s="403" t="s">
         <v>186</v>
       </c>
-      <c r="I17" s="97" t="s">
+      <c r="I17" s="424" t="s">
         <v>89</v>
       </c>
-      <c r="J17" s="97" t="s">
+      <c r="J17" s="445" t="s">
         <v>207</v>
       </c>
-      <c r="K17" s="97" t="s">
+      <c r="K17" s="466" t="s">
         <v>207</v>
       </c>
-      <c r="L17" s="6"/>
+      <c r="L17" s="487" t="s">
+        <v>287</v>
+      </c>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
       <c r="O17" s="6"/>
@@ -21561,32 +23399,34 @@
     <row r="18" spans="1:27" ht="18">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
-      <c r="C18" s="97" t="s">
+      <c r="C18" s="323" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="97" t="s">
+      <c r="D18" s="344" t="s">
         <v>76</v>
       </c>
-      <c r="E18" s="97" t="s">
+      <c r="E18" s="362" t="s">
         <v>149</v>
       </c>
       <c r="F18" s="12"/>
-      <c r="G18" s="97" t="s">
+      <c r="G18" s="383" t="s">
         <v>166</v>
       </c>
-      <c r="H18" s="97" t="s">
+      <c r="H18" s="404" t="s">
         <v>187</v>
       </c>
-      <c r="I18" s="97" t="s">
+      <c r="I18" s="425" t="s">
         <v>89</v>
       </c>
-      <c r="J18" s="97" t="s">
+      <c r="J18" s="446" t="s">
         <v>208</v>
       </c>
-      <c r="K18" s="97" t="s">
+      <c r="K18" s="467" t="s">
         <v>208</v>
       </c>
-      <c r="L18" s="6"/>
+      <c r="L18" s="488" t="s">
+        <v>288</v>
+      </c>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
@@ -21606,32 +23446,34 @@
     <row r="19" spans="1:27" ht="18">
       <c r="A19" s="12"/>
       <c r="B19" s="12"/>
-      <c r="C19" s="97" t="s">
+      <c r="C19" s="324" t="s">
         <v>96</v>
       </c>
-      <c r="D19" s="97" t="s">
+      <c r="D19" s="345" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="97" t="s">
+      <c r="E19" s="363" t="s">
         <v>149</v>
       </c>
       <c r="F19" s="12"/>
-      <c r="G19" s="97" t="s">
+      <c r="G19" s="384" t="s">
         <v>167</v>
       </c>
-      <c r="H19" s="97" t="s">
+      <c r="H19" s="405" t="s">
         <v>188</v>
       </c>
-      <c r="I19" s="97" t="s">
+      <c r="I19" s="426" t="s">
         <v>89</v>
       </c>
-      <c r="J19" s="97" t="s">
+      <c r="J19" s="447" t="s">
         <v>209</v>
       </c>
-      <c r="K19" s="97" t="s">
+      <c r="K19" s="468" t="s">
         <v>209</v>
       </c>
-      <c r="L19" s="6"/>
+      <c r="L19" s="489" t="s">
+        <v>289</v>
+      </c>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
@@ -21651,32 +23493,34 @@
     <row r="20" spans="1:27" ht="18">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
-      <c r="C20" s="97" t="s">
+      <c r="C20" s="325" t="s">
         <v>96</v>
       </c>
-      <c r="D20" s="97" t="s">
+      <c r="D20" s="346" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="97" t="s">
+      <c r="E20" s="364" t="s">
         <v>150</v>
       </c>
       <c r="F20" s="12"/>
-      <c r="G20" s="97" t="s">
+      <c r="G20" s="385" t="s">
         <v>168</v>
       </c>
-      <c r="H20" s="97" t="s">
+      <c r="H20" s="406" t="s">
         <v>189</v>
       </c>
-      <c r="I20" s="97" t="s">
+      <c r="I20" s="427" t="s">
         <v>89</v>
       </c>
-      <c r="J20" s="97" t="s">
+      <c r="J20" s="448" t="s">
         <v>210</v>
       </c>
-      <c r="K20" s="97" t="s">
+      <c r="K20" s="469" t="s">
         <v>210</v>
       </c>
-      <c r="L20" s="6"/>
+      <c r="L20" s="490" t="s">
+        <v>290</v>
+      </c>
       <c r="M20" s="6"/>
       <c r="N20" s="6"/>
       <c r="O20" s="6"/>
@@ -21696,32 +23540,34 @@
     <row r="21" spans="1:27" ht="18">
       <c r="A21" s="12"/>
       <c r="B21" s="12"/>
-      <c r="C21" s="97" t="s">
+      <c r="C21" s="326" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="97" t="s">
+      <c r="D21" s="347" t="s">
         <v>76</v>
       </c>
-      <c r="E21" s="97" t="s">
+      <c r="E21" s="365" t="s">
         <v>150</v>
       </c>
       <c r="F21" s="12"/>
-      <c r="G21" s="97" t="s">
+      <c r="G21" s="386" t="s">
         <v>169</v>
       </c>
-      <c r="H21" s="97" t="s">
+      <c r="H21" s="407" t="s">
         <v>190</v>
       </c>
-      <c r="I21" s="97" t="s">
+      <c r="I21" s="428" t="s">
         <v>89</v>
       </c>
-      <c r="J21" s="97" t="s">
+      <c r="J21" s="449" t="s">
         <v>211</v>
       </c>
-      <c r="K21" s="97" t="s">
+      <c r="K21" s="470" t="s">
         <v>211</v>
       </c>
-      <c r="L21" s="6"/>
+      <c r="L21" s="491" t="s">
+        <v>291</v>
+      </c>
       <c r="M21" s="6"/>
       <c r="N21" s="6"/>
       <c r="O21" s="6"/>
@@ -21741,32 +23587,34 @@
     <row r="22" spans="1:27" ht="18">
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
-      <c r="C22" s="97" t="s">
+      <c r="C22" s="327" t="s">
         <v>96</v>
       </c>
-      <c r="D22" s="97" t="s">
+      <c r="D22" s="348" t="s">
         <v>77</v>
       </c>
-      <c r="E22" s="97" t="s">
+      <c r="E22" s="366" t="s">
         <v>149</v>
       </c>
       <c r="F22" s="12"/>
-      <c r="G22" s="97" t="s">
+      <c r="G22" s="387" t="s">
         <v>170</v>
       </c>
-      <c r="H22" s="97" t="s">
+      <c r="H22" s="408" t="s">
         <v>191</v>
       </c>
-      <c r="I22" s="97" t="s">
+      <c r="I22" s="429" t="s">
         <v>89</v>
       </c>
-      <c r="J22" s="97" t="s">
+      <c r="J22" s="450" t="s">
         <v>212</v>
       </c>
-      <c r="K22" s="97" t="s">
+      <c r="K22" s="471" t="s">
         <v>212</v>
       </c>
-      <c r="L22" s="6"/>
+      <c r="L22" s="492" t="s">
+        <v>292</v>
+      </c>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
@@ -21786,32 +23634,34 @@
     <row r="23" spans="1:27" ht="18">
       <c r="A23" s="12"/>
       <c r="B23" s="12"/>
-      <c r="C23" s="97" t="s">
+      <c r="C23" s="328" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="97" t="s">
+      <c r="D23" s="349" t="s">
         <v>77</v>
       </c>
-      <c r="E23" s="97" t="s">
+      <c r="E23" s="367" t="s">
         <v>150</v>
       </c>
       <c r="F23" s="12"/>
-      <c r="G23" s="97" t="s">
+      <c r="G23" s="388" t="s">
         <v>171</v>
       </c>
-      <c r="H23" s="97" t="s">
+      <c r="H23" s="409" t="s">
         <v>192</v>
       </c>
-      <c r="I23" s="97" t="s">
+      <c r="I23" s="430" t="s">
         <v>89</v>
       </c>
-      <c r="J23" s="97" t="s">
+      <c r="J23" s="451" t="s">
         <v>213</v>
       </c>
-      <c r="K23" s="97" t="s">
+      <c r="K23" s="472" t="s">
         <v>213</v>
       </c>
-      <c r="L23" s="6"/>
+      <c r="L23" s="493" t="s">
+        <v>293</v>
+      </c>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
@@ -24076,20 +25926,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.33203125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.83203125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.5" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="7.1640625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="19.5" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="17.6640625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.5" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="75" width="19.33203125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.1640625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="21.83203125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="28.1640625" collapsed="false"/>
-    <col min="12" max="12" style="75" width="14.5" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" style="75" width="16.6640625" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="21.6640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.83203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.5" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="7.1640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="75" width="19.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.1640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="21.83203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.1640625" collapsed="true"/>
+    <col min="12" max="12" style="75" width="14.5" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="75" width="16.6640625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="21.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="21.75" customHeight="1">
@@ -24169,245 +26019,263 @@
     <row r="3" spans="1:33" ht="17">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="494" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="503" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="512" t="s">
         <v>214</v>
       </c>
-      <c r="F3" s="97" t="s">
+      <c r="F3" s="521" t="s">
         <v>223</v>
       </c>
-      <c r="G3" s="97" t="s">
+      <c r="G3" s="530" t="s">
         <v>89</v>
       </c>
-      <c r="H3" s="97" t="s">
+      <c r="H3" s="539" t="s">
         <v>232</v>
       </c>
       <c r="I3" s="44"/>
       <c r="J3" s="45"/>
       <c r="K3" s="46"/>
-      <c r="L3" s="83"/>
+      <c r="L3" s="548" t="s">
+        <v>294</v>
+      </c>
       <c r="M3" s="84"/>
       <c r="N3" s="47"/>
     </row>
     <row r="4" spans="1:33" ht="17">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="495" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="504" t="s">
         <v>77</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="513" t="s">
         <v>215</v>
       </c>
-      <c r="F4" s="97" t="s">
+      <c r="F4" s="522" t="s">
         <v>224</v>
       </c>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="531" t="s">
         <v>89</v>
       </c>
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="540" t="s">
         <v>233</v>
       </c>
       <c r="I4" s="44"/>
       <c r="J4" s="45"/>
       <c r="K4" s="46"/>
-      <c r="L4" s="83"/>
+      <c r="L4" s="549" t="s">
+        <v>295</v>
+      </c>
       <c r="M4" s="84"/>
     </row>
     <row r="5" spans="1:33" ht="17">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="496" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="505" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="514" t="s">
         <v>216</v>
       </c>
-      <c r="F5" s="97" t="s">
+      <c r="F5" s="523" t="s">
         <v>225</v>
       </c>
-      <c r="G5" s="97" t="s">
+      <c r="G5" s="532" t="s">
         <v>89</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="541" t="s">
         <v>234</v>
       </c>
       <c r="I5" s="44"/>
       <c r="J5" s="48"/>
       <c r="K5" s="46"/>
-      <c r="L5" s="83"/>
+      <c r="L5" s="550" t="s">
+        <v>296</v>
+      </c>
       <c r="M5" s="84"/>
     </row>
     <row r="6" spans="1:33" ht="17">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="497" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="506" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="97" t="s">
+      <c r="E6" s="515" t="s">
         <v>217</v>
       </c>
-      <c r="F6" s="97" t="s">
+      <c r="F6" s="524" t="s">
         <v>226</v>
       </c>
-      <c r="G6" s="97" t="s">
+      <c r="G6" s="533" t="s">
         <v>89</v>
       </c>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="542" t="s">
         <v>235</v>
       </c>
       <c r="I6" s="44"/>
       <c r="J6" s="49"/>
       <c r="K6" s="46"/>
-      <c r="L6" s="83"/>
+      <c r="L6" s="551" t="s">
+        <v>297</v>
+      </c>
       <c r="M6" s="84"/>
     </row>
     <row r="7" spans="1:33" ht="17">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="97" t="s">
+      <c r="C7" s="498" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="507" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="516" t="s">
         <v>218</v>
       </c>
-      <c r="F7" s="97" t="s">
+      <c r="F7" s="525" t="s">
         <v>227</v>
       </c>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="534" t="s">
         <v>89</v>
       </c>
-      <c r="H7" s="97" t="s">
+      <c r="H7" s="543" t="s">
         <v>236</v>
       </c>
       <c r="I7" s="44"/>
       <c r="J7" s="45"/>
       <c r="K7" s="46"/>
-      <c r="L7" s="83"/>
+      <c r="L7" s="552" t="s">
+        <v>298</v>
+      </c>
       <c r="M7" s="84"/>
     </row>
     <row r="8" spans="1:33" ht="17">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="97" t="s">
+      <c r="C8" s="499" t="s">
         <v>95</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="508" t="s">
         <v>76</v>
       </c>
-      <c r="E8" s="97" t="s">
+      <c r="E8" s="517" t="s">
         <v>219</v>
       </c>
-      <c r="F8" s="97" t="s">
+      <c r="F8" s="526" t="s">
         <v>228</v>
       </c>
-      <c r="G8" s="97" t="s">
+      <c r="G8" s="535" t="s">
         <v>89</v>
       </c>
-      <c r="H8" s="97" t="s">
+      <c r="H8" s="544" t="s">
         <v>237</v>
       </c>
       <c r="I8" s="44"/>
       <c r="J8" s="45"/>
       <c r="K8" s="46"/>
-      <c r="L8" s="83"/>
+      <c r="L8" s="553" t="s">
+        <v>299</v>
+      </c>
       <c r="M8" s="84"/>
     </row>
     <row r="9" spans="1:33" ht="17">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="97" t="s">
+      <c r="C9" s="500" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="97" t="s">
+      <c r="D9" s="509" t="s">
         <v>77</v>
       </c>
-      <c r="E9" s="97" t="s">
+      <c r="E9" s="518" t="s">
         <v>220</v>
       </c>
-      <c r="F9" s="97" t="s">
+      <c r="F9" s="527" t="s">
         <v>229</v>
       </c>
-      <c r="G9" s="97" t="s">
+      <c r="G9" s="536" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="97" t="s">
+      <c r="H9" s="545" t="s">
         <v>238</v>
       </c>
       <c r="I9" s="44"/>
       <c r="J9" s="45"/>
       <c r="K9" s="46"/>
-      <c r="L9" s="83"/>
+      <c r="L9" s="554" t="s">
+        <v>300</v>
+      </c>
       <c r="M9" s="84"/>
     </row>
     <row r="10" spans="1:33" ht="17">
       <c r="A10" s="12"/>
       <c r="B10" s="12"/>
-      <c r="C10" s="97" t="s">
+      <c r="C10" s="501" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="97" t="s">
+      <c r="D10" s="510" t="s">
         <v>76</v>
       </c>
-      <c r="E10" s="97" t="s">
+      <c r="E10" s="519" t="s">
         <v>221</v>
       </c>
-      <c r="F10" s="97" t="s">
+      <c r="F10" s="528" t="s">
         <v>230</v>
       </c>
-      <c r="G10" s="97" t="s">
+      <c r="G10" s="537" t="s">
         <v>89</v>
       </c>
-      <c r="H10" s="97" t="s">
+      <c r="H10" s="546" t="s">
         <v>239</v>
       </c>
       <c r="I10" s="44"/>
       <c r="J10" s="45"/>
       <c r="K10" s="46"/>
-      <c r="L10" s="83"/>
+      <c r="L10" s="555" t="s">
+        <v>301</v>
+      </c>
       <c r="M10" s="84"/>
     </row>
     <row r="11" spans="1:33" ht="17">
       <c r="A11" s="16"/>
       <c r="B11" s="12"/>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="502" t="s">
         <v>94</v>
       </c>
-      <c r="D11" s="97" t="s">
+      <c r="D11" s="511" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="97" t="s">
+      <c r="E11" s="520" t="s">
         <v>222</v>
       </c>
-      <c r="F11" s="97" t="s">
+      <c r="F11" s="529" t="s">
         <v>231</v>
       </c>
-      <c r="G11" s="97" t="s">
+      <c r="G11" s="538" t="s">
         <v>89</v>
       </c>
-      <c r="H11" s="97" t="s">
+      <c r="H11" s="547" t="s">
         <v>240</v>
       </c>
       <c r="I11" s="44"/>
       <c r="J11" s="48"/>
       <c r="K11" s="46"/>
-      <c r="L11" s="83"/>
+      <c r="L11" s="556" t="s">
+        <v>302</v>
+      </c>
       <c r="M11" s="84"/>
     </row>
     <row r="12" spans="1:33" ht="15.75" customHeight="1">
@@ -26036,19 +27904,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.5" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="12.5" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.33203125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="9.5" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="10.33203125" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="22.5" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="17.5" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.5" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" style="75" width="17.0" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="16.5" collapsed="false"/>
-    <col min="12" max="13" customWidth="true" width="10.83203125" collapsed="false"/>
-    <col min="14" max="31" customWidth="true" width="10.6640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="22.5" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="17.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="75" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="12" max="13" customWidth="true" width="10.83203125" collapsed="true"/>
+    <col min="14" max="31" customWidth="true" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18.75" customHeight="1">
@@ -26124,30 +27992,32 @@
     <row r="3" spans="1:31" ht="18">
       <c r="A3" s="12"/>
       <c r="B3" s="12"/>
-      <c r="C3" s="97" t="s">
+      <c r="C3" s="557" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="97" t="s">
+      <c r="D3" s="563" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="97" t="s">
+      <c r="E3" s="569" t="s">
         <v>150</v>
       </c>
       <c r="F3" s="12"/>
-      <c r="G3" s="97" t="s">
+      <c r="G3" s="575" t="s">
         <v>241</v>
       </c>
-      <c r="H3" s="97" t="s">
+      <c r="H3" s="581" t="s">
         <v>245</v>
       </c>
-      <c r="I3" s="97" t="s">
+      <c r="I3" s="587" t="s">
         <v>89</v>
       </c>
-      <c r="J3" s="97" t="s">
+      <c r="J3" s="593" t="s">
         <v>251</v>
       </c>
       <c r="K3" s="55"/>
-      <c r="L3" s="6"/>
+      <c r="L3" s="599" t="s">
+        <v>303</v>
+      </c>
       <c r="M3" s="6"/>
       <c r="N3" s="6"/>
       <c r="O3" s="6"/>
@@ -26169,30 +28039,32 @@
     <row r="4" spans="1:31" ht="18">
       <c r="A4" s="12"/>
       <c r="B4" s="12"/>
-      <c r="C4" s="97" t="s">
+      <c r="C4" s="558" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="97" t="s">
+      <c r="D4" s="564" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="97" t="s">
+      <c r="E4" s="570" t="s">
         <v>149</v>
       </c>
       <c r="F4" s="12"/>
-      <c r="G4" s="97" t="s">
+      <c r="G4" s="576" t="s">
         <v>242</v>
       </c>
-      <c r="H4" s="97" t="s">
+      <c r="H4" s="582" t="s">
         <v>246</v>
       </c>
-      <c r="I4" s="97" t="s">
+      <c r="I4" s="588" t="s">
         <v>89</v>
       </c>
-      <c r="J4" s="97" t="s">
+      <c r="J4" s="594" t="s">
         <v>252</v>
       </c>
       <c r="K4" s="56"/>
-      <c r="L4" s="6"/>
+      <c r="L4" s="600" t="s">
+        <v>304</v>
+      </c>
       <c r="M4" s="6"/>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
@@ -26214,30 +28086,32 @@
     <row r="5" spans="1:31" ht="18">
       <c r="A5" s="12"/>
       <c r="B5" s="12"/>
-      <c r="C5" s="97" t="s">
+      <c r="C5" s="559" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="97" t="s">
+      <c r="D5" s="565" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="97" t="s">
+      <c r="E5" s="571" t="s">
         <v>150</v>
       </c>
       <c r="F5" s="12"/>
-      <c r="G5" s="97" t="s">
+      <c r="G5" s="577" t="s">
         <v>243</v>
       </c>
-      <c r="H5" s="97" t="s">
+      <c r="H5" s="583" t="s">
         <v>247</v>
       </c>
-      <c r="I5" s="97" t="s">
+      <c r="I5" s="589" t="s">
         <v>89</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="595" t="s">
         <v>253</v>
       </c>
       <c r="K5" s="56"/>
-      <c r="L5" s="6"/>
+      <c r="L5" s="601" t="s">
+        <v>305</v>
+      </c>
       <c r="M5" s="6"/>
       <c r="N5" s="6"/>
       <c r="O5" s="6"/>
@@ -26259,30 +28133,32 @@
     <row r="6" spans="1:31" ht="18">
       <c r="A6" s="12"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="97" t="s">
+      <c r="C6" s="560" t="s">
         <v>95</v>
       </c>
-      <c r="D6" s="97" t="s">
+      <c r="D6" s="566" t="s">
         <v>78</v>
       </c>
-      <c r="E6" s="97" t="s">
+      <c r="E6" s="572" t="s">
         <v>149</v>
       </c>
       <c r="F6" s="12"/>
-      <c r="G6" s="97" t="s">
+      <c r="G6" s="578" t="s">
         <v>242</v>
       </c>
-      <c r="H6" s="97" t="s">
+      <c r="H6" s="584" t="s">
         <v>248</v>
       </c>
-      <c r="I6" s="97" t="s">
+      <c r="I6" s="590" t="s">
         <v>89</v>
       </c>
-      <c r="J6" s="97" t="s">
+      <c r="J6" s="596" t="s">
         <v>254</v>
       </c>
       <c r="K6" s="56"/>
-      <c r="L6" s="6"/>
+      <c r="L6" s="602" t="s">
+        <v>306</v>
+      </c>
       <c r="M6" s="6"/>
       <c r="N6" s="6"/>
       <c r="O6" s="6"/>
@@ -26304,30 +28180,32 @@
     <row r="7" spans="1:31" ht="18">
       <c r="A7" s="12"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="97" t="s">
+      <c r="C7" s="561" t="s">
         <v>94</v>
       </c>
-      <c r="D7" s="97" t="s">
+      <c r="D7" s="567" t="s">
         <v>78</v>
       </c>
-      <c r="E7" s="97" t="s">
+      <c r="E7" s="573" t="s">
         <v>150</v>
       </c>
       <c r="F7" s="12"/>
-      <c r="G7" s="97" t="s">
+      <c r="G7" s="579" t="s">
         <v>244</v>
       </c>
-      <c r="H7" s="97" t="s">
+      <c r="H7" s="585" t="s">
         <v>249</v>
       </c>
-      <c r="I7" s="97" t="s">
+      <c r="I7" s="591" t="s">
         <v>89</v>
       </c>
-      <c r="J7" s="97" t="s">
+      <c r="J7" s="597" t="s">
         <v>255</v>
       </c>
       <c r="K7" s="55"/>
-      <c r="L7" s="6"/>
+      <c r="L7" s="603" t="s">
+        <v>307</v>
+      </c>
       <c r="M7" s="6"/>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -26349,30 +28227,32 @@
     <row r="8" spans="1:31" ht="18">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
-      <c r="C8" s="97" t="s">
+      <c r="C8" s="562" t="s">
         <v>94</v>
       </c>
-      <c r="D8" s="97" t="s">
+      <c r="D8" s="568" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="97" t="s">
+      <c r="E8" s="574" t="s">
         <v>149</v>
       </c>
       <c r="F8" s="12"/>
-      <c r="G8" s="97" t="s">
+      <c r="G8" s="580" t="s">
         <v>242</v>
       </c>
-      <c r="H8" s="97" t="s">
+      <c r="H8" s="586" t="s">
         <v>250</v>
       </c>
-      <c r="I8" s="97" t="s">
+      <c r="I8" s="592" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="97" t="s">
+      <c r="J8" s="598" t="s">
         <v>256</v>
       </c>
       <c r="K8" s="55"/>
-      <c r="L8" s="6"/>
+      <c r="L8" s="604" t="s">
+        <v>308</v>
+      </c>
       <c r="M8" s="6"/>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -29281,15 +31161,15 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="8.33203125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="10.33203125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="8.83203125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="15.5" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="57.0" collapsed="false"/>
-    <col min="6" max="7" customWidth="true" width="14.33203125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="20.5" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="false"/>
-    <col min="10" max="11" customWidth="true" width="16.33203125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="8.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.83203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="57.0" collapsed="true"/>
+    <col min="6" max="7" customWidth="true" width="14.33203125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="10" max="11" customWidth="true" width="16.33203125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="18" customHeight="1">
@@ -34773,8 +36653,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="150.0" collapsed="false"/>
-    <col min="2" max="6" customWidth="true" width="10.6640625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="150.0" collapsed="true"/>
+    <col min="2" max="6" customWidth="true" width="10.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="26.25" customHeight="1">

</xml_diff>